<commit_message>
Moving identified missing TM5 variables to the basic identified missing file (related to #83) and update/unify the comments column
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="499">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -881,6 +881,642 @@
   </si>
   <si>
     <t xml:space="preserve">fVegSoil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude plev19 time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mole Fraction of O3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This TM5  variable name equals the cmor name. Postprocessing in ece2cmor3 has to be added.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tommi Bergman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mole Fraction of CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ch4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mole Fraction of CH4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude alevhalf time2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phalf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure on Model Half-Levels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6hrLev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude alevel time1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ec550aer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerosol extinction coefficient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AERhr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sfno2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO2 volume mixing ratio in lowest model layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sfo3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O3 volume mixing ratio in lowest model layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sfpm25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM2.5 mass mixing ratio in lowest model layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AERmon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abs550aer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ambient aerosol absorption optical thickness at 550 nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude alevel time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">airmass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically integrated mass content of air in layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bldep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boundary Layer Depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c2h6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2H6 volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c3h6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3H6  volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c3h8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3H8  volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ch3coch3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH3COCH3  volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH4 volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cheaqpso4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aqueous-phase production rate of SO4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chegpso4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas-phase production rate of SO4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chepsoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chemical production of dry aerosol secondary organic matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2 volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMS volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drybc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dry deposition rate of black carbon aerosol mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drydust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dry deposition rate of dust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drynh3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dry deposition rate of nh3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drynh4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dry deposition rate of nh4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drynoy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dry deposition rate of noy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dryo3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dry deposition rate of o3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dryoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dry deposition rate of dry aerosol total organic matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dryso2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dry deposition rate of so2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dryso4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dry deposition rate of so4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dryss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dry deposition rate of seasalt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emibc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emission rate of black carbon aerosol mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total emission rate of co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emidms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total emission rate of dms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emidust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total emission rate of dust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emiisop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total emission rate of isoprene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emilnox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">layer-integrated lightning production of NOx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eminh3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total emission rate of nh3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eminox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total emission rate of nox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emioa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">primary emission and chemical production of dry aerosol organic matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emiso2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total emission rate of so2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emiso4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total direct emission rate of so4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emiss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total emission rate of seasalt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h2o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass Fraction of Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hno3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HNO3 volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isoprene volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jno2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">photolysis rate of NO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmraerh2o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerosol water mass mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmrbc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elemental carbon mass mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmrdust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dust aerosol mass mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmrnh4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NH4 mass mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmrno3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO3 aerosol mass mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmroa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total organic aerosol mass mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmrpm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM1.0 mass mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmrpm10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM10 mass mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmrpm2p5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM2.5 mass mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmrso4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerosol sulfate mass mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmrsoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary organic aerosol mass mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmrss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sea Salt mass mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nh50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artificial tracer with 50 day lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO2 volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ozone volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od440aer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ambient aerosol optical thickness at 440 nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od550aer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ambient aerosol optical thickness at 550 nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od550aerh2o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aerosol water aod@550nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od550bc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">black carbon aod@550nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od550csaer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od550dust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dust aod@550nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od550lt1aer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ambient fine mode aerosol optical thickness at 550 nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od550no3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nitrate aod@550nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od550oa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total organic aerosol aod@550nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od550so4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sulfate aod@550nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od550soa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soa aod@550nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od550ss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sea salt aod@550nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od870aer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ambient aerosol optical thickness at 870 nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OH volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAN volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude alevhalf time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tropopause Air Pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">so2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SO2 volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tatp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tropopause Air Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Ozone Column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tropoz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tropospheric ozone column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wetbc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wet deposition rate of black carbon aerosol mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wetdust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wet deposition rate of dust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wetnh3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wet deposition rate of nh3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wetnh4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wet deposition rate of nh4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wetnoy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wet deposition of noy incl aerosol nitrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wetoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wet deposition rate of dry aerosol total organic matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wetso2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wet deposition rate of so2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wetso4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wet deposition rate of so4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wetss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wet deposition rate of seasalt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tropopause Altitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AERday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maxpblz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maximum PBL height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minpblz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimum PBL height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sfo3max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">daily maximum O3 volume mixing ratio in lowest model layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Column Ozone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CFsubhr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alevhalf site time1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AERmonZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latitude plev39 time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ho2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HO2 volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total reactive nitrogen volume mixing ratio</t>
   </si>
 </sst>
 </file>
@@ -964,7 +1600,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -975,6 +1611,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -994,13 +1634,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F290"/>
+  <dimension ref="A1:F414"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D232" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3:E255"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A387" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E408" activeCellId="0" sqref="E408:E414"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.71"/>
@@ -4089,6 +4729,2166 @@
         <v>263</v>
       </c>
     </row>
+    <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B301" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="C301" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="D301" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="E301" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F301" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B302" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="C302" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="D302" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="E302" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F302" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B303" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="C303" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="D303" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="E303" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F303" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B304" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="C304" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="D304" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="E304" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F304" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B306" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C306" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="D306" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="E306" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F306" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B308" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C308" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="D308" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="E308" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F308" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B309" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C309" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="D309" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="E309" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F309" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B310" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C310" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="D310" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="E310" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F310" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A312" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B312" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C312" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="D312" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="E312" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F312" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B313" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C313" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="D313" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="E313" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F313" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B314" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C314" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="D314" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="E314" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F314" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B315" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C315" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="D315" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="E315" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F315" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B316" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C316" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="D316" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="E316" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F316" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B317" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C317" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="D317" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="E317" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F317" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B318" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C318" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="D318" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="E318" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F318" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A319" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B319" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C319" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="D319" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="E319" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F319" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B320" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C320" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="D320" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="E320" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F320" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B321" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C321" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="D321" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="E321" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F321" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B322" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C322" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="D322" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E322" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F322" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B323" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C323" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="D323" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="E323" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F323" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B324" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C324" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="D324" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="E324" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F324" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B325" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C325" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="D325" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="E325" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F325" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B326" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C326" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="D326" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="E326" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F326" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B327" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C327" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="D327" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="E327" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F327" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B328" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C328" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="D328" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="E328" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F328" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B329" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C329" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="D329" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="E329" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F329" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B330" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C330" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="D330" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="E330" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F330" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B331" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C331" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="D331" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="E331" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F331" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B332" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C332" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="D332" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="E332" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F332" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A333" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B333" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C333" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="D333" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="E333" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F333" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B334" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C334" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="D334" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="E334" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F334" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B335" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C335" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="D335" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="E335" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F335" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B336" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C336" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="D336" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="E336" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F336" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B337" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C337" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="D337" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="E337" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F337" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B338" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C338" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="D338" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="E338" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F338" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B339" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C339" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="D339" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E339" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F339" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B340" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C340" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="D340" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="E340" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F340" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B341" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C341" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="D341" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="E341" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F341" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B342" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C342" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="D342" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="E342" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F342" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B343" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C343" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="D343" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="E343" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F343" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A344" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B344" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C344" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="D344" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="E344" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F344" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B345" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C345" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="D345" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="E345" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F345" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B346" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C346" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="D346" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="E346" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F346" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B347" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C347" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="D347" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="E347" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F347" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B348" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C348" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="D348" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="E348" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F348" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A349" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B349" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C349" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="D349" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="E349" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F349" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A350" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B350" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C350" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="D350" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="E350" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F350" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B351" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C351" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="D351" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="E351" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F351" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A352" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B352" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C352" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="D352" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="E352" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F352" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A353" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B353" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C353" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="D353" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="E353" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F353" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A354" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B354" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C354" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="D354" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="E354" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F354" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B355" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C355" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="D355" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="E355" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F355" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A356" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B356" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C356" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="D356" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="E356" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F356" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B357" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C357" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="D357" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="E357" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F357" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A358" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B358" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C358" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="D358" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="E358" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F358" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B359" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C359" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="D359" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="E359" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F359" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B360" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C360" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="D360" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="E360" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F360" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A361" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B361" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C361" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D361" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="E361" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F361" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B362" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C362" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="D362" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="E362" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F362" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B363" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C363" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="D363" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="E363" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F363" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A364" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B364" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C364" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="D364" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="E364" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F364" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B365" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C365" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="D365" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="E365" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F365" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A366" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B366" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C366" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="D366" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="E366" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F366" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A367" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B367" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C367" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="D367" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="E367" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F367" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A368" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B368" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C368" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="D368" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="E368" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F368" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A369" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B369" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C369" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="D369" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="E369" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F369" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A370" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B370" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C370" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="D370" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="E370" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F370" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A371" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B371" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C371" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="D371" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="E371" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F371" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A372" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B372" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C372" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="D372" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="E372" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F372" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A373" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B373" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C373" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="D373" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="E373" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F373" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A374" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B374" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C374" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="D374" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="E374" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F374" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A375" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B375" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C375" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="D375" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="E375" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F375" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A376" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B376" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C376" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="D376" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="E376" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F376" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A377" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B377" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C377" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="D377" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="E377" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F377" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A378" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B378" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C378" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="D378" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="E378" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F378" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A379" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B379" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C379" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="D379" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="E379" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F379" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A380" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B380" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C380" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="D380" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="E380" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F380" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A381" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B381" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C381" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="D381" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="E381" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F381" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A382" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B382" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C382" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="D382" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="E382" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F382" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A383" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B383" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="C383" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="D383" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="E383" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F383" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A384" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B384" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C384" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="D384" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="E384" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F384" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A385" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B385" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C385" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="D385" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="E385" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F385" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A386" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B386" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C386" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="D386" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="E386" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F386" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A387" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B387" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C387" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="D387" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="E387" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F387" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A388" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B388" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C388" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="D388" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="E388" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F388" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A389" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B389" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C389" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="D389" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="E389" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F389" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A390" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B390" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C390" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="D390" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="E390" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F390" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A391" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B391" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C391" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="D391" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="E391" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F391" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A392" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B392" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C392" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="D392" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="E392" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F392" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A393" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B393" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C393" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="D393" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="E393" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F393" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A394" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B394" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C394" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="D394" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="E394" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F394" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A395" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B395" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C395" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D395" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="E395" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F395" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A396" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B396" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C396" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="D396" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="E396" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F396" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A397" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B397" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C397" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="D397" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="E397" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F397" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A398" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B398" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C398" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="D398" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="E398" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F398" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A400" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="B400" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C400" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="D400" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="E400" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F400" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A401" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="B401" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C401" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="D401" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="E401" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F401" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A402" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="B402" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C402" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="D402" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="E402" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F402" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A403" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="B403" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C403" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D403" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="E403" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F403" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A404" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="B404" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C404" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="D404" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="E404" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F404" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A406" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="B406" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="C406" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="D406" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="E406" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F406" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A408" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B408" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C408" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="D408" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="E408" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F408" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A409" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B409" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C409" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="D409" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="E409" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F409" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A410" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B410" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C410" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="D410" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="E410" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F410" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A411" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B411" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C411" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="D411" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="E411" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F411" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A412" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B412" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C412" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="D412" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="E412" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F412" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A413" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B413" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C413" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="D413" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="E413" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F413" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A414" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B414" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C414" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="D414" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="E414" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F414" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Two TM5 variables have been identified by Tommi Bergman, updating for that.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="503">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -1517,6 +1517,18 @@
   </si>
   <si>
     <t xml:space="preserve">Total reactive nitrogen volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emibvoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total emission rate of biogenic nmvoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emivoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total emission rate of nmvoc</t>
   </si>
 </sst>
 </file>
@@ -1634,10 +1646,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F414"/>
+  <dimension ref="A1:F417"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A387" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E408" activeCellId="0" sqref="E408:E414"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A384" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E417" activeCellId="0" sqref="E417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6889,6 +6901,46 @@
         <v>292</v>
       </c>
     </row>
+    <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A416" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B416" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C416" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="D416" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="E416" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F416" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A417" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B417" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C417" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="D417" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="E417" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F417" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update basic identified missing and basic ignored files #96
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="532">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -1529,6 +1529,93 @@
   </si>
   <si>
     <t xml:space="preserve">total emission rate of nmvoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fco2antt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon Mass Flux into Atmosphere Due to All Anthropogenic Emissions of CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in the AOGCM, but will be added by Tommi  in the ESM in TM5 with its cmor name.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is requested only for the emission-driven coupled carbon climate model runs.  Does not include natural fire sources but, includes all anthropogenic sources, including fossil fuel use, cement production, agricultural burning, and sources associated with anthropogenic land use change excluding forest regrowth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fco2fos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon Mass Flux into Atmosphere Due to Fossil Fuel Emissions of CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the prescribed anthropogenic CO2 flux from fossil fuel use, including cement production, and flaring (but not from land-use changes, agricultural burning, forest regrowth, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fco2nat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Carbon Mass Flux into the Atmosphere Due to Natural Sources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is what the atmosphere sees (on its own grid).  This field should be equivalent to the combined natural fluxes of carbon  that account for natural exchanges between the atmosphere and land (nep) or ocean (fgco2) reservoirs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude plev19 time2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o3Clim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co2Clim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co2mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Atmospheric Mass of CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total atmospheric mass of Carbon Dioxide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co2massClim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ch4Clim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ch4global</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global Mean Mole Fraction of CH4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ch4globalClim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n2oClim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mole Fraction of N2O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n2oglobal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global Mean Mole Fraction of N2O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global mean Nitrous Oxide (N2O)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n2oglobalClim</t>
   </si>
 </sst>
 </file>
@@ -1646,10 +1733,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F417"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A384" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E417" activeCellId="0" sqref="E417"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D411" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F419" activeCellId="0" sqref="F419:F431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6941,6 +7028,296 @@
         <v>292</v>
       </c>
     </row>
+    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A419" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B419" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C419" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="D419" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="E419" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="F419" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="H419" s="0" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A420" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B420" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C420" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="D420" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="E420" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="F420" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="H420" s="0" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A421" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B421" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C421" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="D421" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="E421" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="F421" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="H421" s="0" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A422" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B422" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C422" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="D422" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="E422" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="F422" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A423" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B423" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C423" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="D423" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="E423" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="F423" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A424" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B424" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="C424" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="D424" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="E424" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="F424" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="H424" s="0" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A425" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B425" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="C425" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="D425" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="E425" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="F425" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="H425" s="0" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A426" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B426" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C426" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="D426" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="E426" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="F426" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A427" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B427" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="C427" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="D427" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="E427" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="F427" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="H427" s="0" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A428" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B428" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="C428" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="D428" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="E428" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="F428" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="H428" s="0" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A429" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B429" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C429" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="D429" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="E429" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="F429" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A430" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B430" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="C430" s="0" t="s">
+        <v>528</v>
+      </c>
+      <c r="D430" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="E430" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="F430" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="H430" s="0" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A431" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B431" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="C431" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="D431" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="E431" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="F431" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="H431" s="0" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Add four more LPJ_GUESS related variables to the identified missing file.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="546">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -883,6 +883,51 @@
     <t xml:space="preserve">fVegSoil</t>
   </si>
   <si>
+    <t xml:space="preserve">Emon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cSoil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon Mass in Soil Pool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon mass in the full depth of the soil model.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude sdepth time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrsol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total water content of soil layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in each soil layer, the mass of water in all phases, including ice.  Reported as 'missing' for grid cells occupied entirely by 'sea'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Carbon Mass Flux out of Atmophere due to Net Ecosystem Productivity on Land.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natural flux of CO2 (expressed as a mass flux of carbon) from the atmosphere to the land calculated as the difference between uptake associated will photosynthesis and the release of CO2 from the sum of plant and soil respiration and fire.  Positive flux is into the land.  emissions from natural fires and human ignition fires as calculated by the fire module of the dynamic vegetation model, but excluding any CO2 flux from fire included in fLuc (CO2 Flux to Atmosphere from Land Use Change).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fLuc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Carbon Mass Flux into Atmosphere due to Land Use Change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon mass flux per unit area into atmosphere due to human changes to land (excluding forest regrowth) accounting possibly for different time-scales related to fate of the wood, for example.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Amon</t>
   </si>
   <si>
@@ -935,9 +980,6 @@
   </si>
   <si>
     <t xml:space="preserve">AERhr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time</t>
   </si>
   <si>
     <t xml:space="preserve">sfno2</t>
@@ -1733,10 +1775,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H435"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D411" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F419" activeCellId="0" sqref="F419:F431"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A279" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A298" activeCellId="0" sqref="298:298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4828,2496 +4870,2585 @@
         <v>263</v>
       </c>
     </row>
-    <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="0" t="s">
+    <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="0" t="s">
         <v>287</v>
       </c>
-      <c r="B301" s="0" t="s">
+      <c r="B292" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="C301" s="0" t="s">
+      <c r="C292" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="D301" s="0" t="s">
+      <c r="D292" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="E301" s="0" t="s">
+      <c r="E292" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="F292" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="H292" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="F301" s="3" t="s">
+    </row>
+    <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B293" s="0" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="0" t="s">
+      <c r="C293" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="D293" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="E293" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="F293" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="H293" s="0" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="0" t="s">
         <v>287</v>
       </c>
-      <c r="B302" s="0" t="s">
+      <c r="B294" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="C302" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="D302" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="E302" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="F302" s="3" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="0" t="s">
+      <c r="C294" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="D294" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="E294" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="F294" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="H294" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="0" t="s">
         <v>287</v>
       </c>
-      <c r="B303" s="0" t="s">
+      <c r="B295" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="C303" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="D303" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="E303" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="F303" s="3" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="B304" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="C304" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="D304" s="0" t="s">
+      <c r="C295" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="E304" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="F304" s="3" t="s">
-        <v>292</v>
+      <c r="D295" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="E295" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="F295" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="H295" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B305" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="C305" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="D305" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="E305" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F305" s="3" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B306" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C306" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="D306" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="E306" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F306" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="D306" s="0" t="s">
+      <c r="B307" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="E306" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="F306" s="0" t="s">
-        <v>292</v>
+      <c r="C307" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="D307" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="E307" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F307" s="3" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B308" s="0" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="C308" s="0" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="D308" s="0" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="E308" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="F308" s="0" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="B309" s="0" t="s">
-        <v>305</v>
-      </c>
-      <c r="C309" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="D309" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="E309" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="F309" s="0" t="s">
-        <v>292</v>
+        <v>306</v>
+      </c>
+      <c r="F308" s="3" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="B310" s="0" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
       <c r="C310" s="0" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="D310" s="0" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="E310" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F310" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="B312" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C312" s="0" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="D312" s="0" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="E312" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F312" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="0" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="B313" s="0" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="C313" s="0" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="D313" s="0" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="E313" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F313" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="B314" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C314" s="0" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="D314" s="0" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="E314" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F314" s="0" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="B315" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="C315" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="D315" s="0" t="s">
-        <v>321</v>
-      </c>
-      <c r="E315" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="F315" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B316" s="0" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="C316" s="0" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="D316" s="0" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="E316" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F316" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B317" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C317" s="0" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="D317" s="0" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="E317" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F317" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B318" s="0" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="C318" s="0" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="D318" s="0" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="E318" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F318" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B319" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C319" s="0" t="s">
-        <v>295</v>
+        <v>334</v>
       </c>
       <c r="D319" s="0" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="E319" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F319" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B320" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C320" s="0" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="D320" s="0" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="E320" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F320" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B321" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C321" s="0" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="D321" s="0" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="E321" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F321" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B322" s="0" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
       <c r="C322" s="0" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="D322" s="0" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="E322" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F322" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B323" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C323" s="0" t="s">
-        <v>335</v>
+        <v>310</v>
       </c>
       <c r="D323" s="0" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="E323" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F323" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B324" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C324" s="0" t="s">
-        <v>293</v>
+        <v>343</v>
       </c>
       <c r="D324" s="0" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="E324" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F324" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B325" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C325" s="0" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="D325" s="0" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="E325" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F325" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B326" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C326" s="0" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="D326" s="0" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="E326" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F326" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B327" s="0" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
       <c r="C327" s="0" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="D327" s="0" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="E327" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F327" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B328" s="0" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
       <c r="C328" s="0" t="s">
-        <v>344</v>
+        <v>308</v>
       </c>
       <c r="D328" s="0" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="E328" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F328" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B329" s="0" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
       <c r="C329" s="0" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="D329" s="0" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="E329" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F329" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B330" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C330" s="0" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="D330" s="0" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="E330" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F330" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B331" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C331" s="0" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="D331" s="0" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="E331" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F331" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B332" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C332" s="0" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="D332" s="0" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="E332" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F332" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B333" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C333" s="0" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="D333" s="0" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="E333" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F333" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B334" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C334" s="0" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="D334" s="0" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="E334" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F334" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B335" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C335" s="0" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="D335" s="0" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="E335" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F335" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B336" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C336" s="0" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="D336" s="0" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="E336" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F336" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B337" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C337" s="0" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="D337" s="0" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="E337" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F337" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B338" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C338" s="0" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="D338" s="0" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="E338" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F338" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B339" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C339" s="0" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="D339" s="0" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="E339" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F339" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B340" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C340" s="0" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="D340" s="0" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="E340" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F340" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B341" s="0" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="C341" s="0" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="D341" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="E341" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F341" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B342" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C342" s="0" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="D342" s="0" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="E342" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F342" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B343" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C343" s="0" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="D343" s="0" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="E343" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F343" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B344" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C344" s="0" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="D344" s="0" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="E344" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F344" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B345" s="0" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
       <c r="C345" s="0" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="D345" s="0" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="E345" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F345" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B346" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C346" s="0" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="D346" s="0" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="E346" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F346" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B347" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C347" s="0" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="D347" s="0" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="E347" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F347" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B348" s="0" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="C348" s="0" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="D348" s="0" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="E348" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F348" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B349" s="0" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="C349" s="0" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="D349" s="0" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="E349" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F349" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B350" s="0" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="C350" s="0" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="D350" s="0" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="E350" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F350" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B351" s="0" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="C351" s="0" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="D351" s="0" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="E351" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F351" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B352" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C352" s="0" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="D352" s="0" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="E352" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F352" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B353" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C353" s="0" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="D353" s="0" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="E353" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F353" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B354" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C354" s="0" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="D354" s="0" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="E354" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F354" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B355" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C355" s="0" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="D355" s="0" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="E355" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F355" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B356" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C356" s="0" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="D356" s="0" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="E356" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F356" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B357" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C357" s="0" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="D357" s="0" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="E357" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F357" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B358" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C358" s="0" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="D358" s="0" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="E358" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F358" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B359" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C359" s="0" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="D359" s="0" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="E359" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F359" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B360" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C360" s="0" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="D360" s="0" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="E360" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F360" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B361" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C361" s="0" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="D361" s="0" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="E361" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F361" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B362" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C362" s="0" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="D362" s="0" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="E362" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F362" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B363" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C363" s="0" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="D363" s="0" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="E363" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F363" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B364" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C364" s="0" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="D364" s="0" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="E364" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F364" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B365" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C365" s="0" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="D365" s="0" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="E365" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F365" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B366" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C366" s="0" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="D366" s="0" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="E366" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F366" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B367" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C367" s="0" t="s">
-        <v>289</v>
+        <v>428</v>
       </c>
       <c r="D367" s="0" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="E367" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F367" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B368" s="0" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
       <c r="C368" s="0" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="D368" s="0" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="E368" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F368" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B369" s="0" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
       <c r="C369" s="0" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
       <c r="D369" s="0" t="s">
-        <v>426</v>
+        <v>433</v>
       </c>
       <c r="E369" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F369" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B370" s="0" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
       <c r="C370" s="0" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="D370" s="0" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="E370" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F370" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B371" s="0" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
       <c r="C371" s="0" t="s">
-        <v>429</v>
+        <v>304</v>
       </c>
       <c r="D371" s="0" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="E371" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F371" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B372" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C372" s="0" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="D372" s="0" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
       <c r="E372" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F372" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B373" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C373" s="0" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="D373" s="0" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="E373" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F373" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B374" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C374" s="0" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="D374" s="0" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="E374" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F374" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B375" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C375" s="0" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="D375" s="0" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="E375" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F375" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B376" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C376" s="0" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="D376" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E376" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F376" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B377" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C377" s="0" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="D377" s="0" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E377" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F377" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B378" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C378" s="0" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="D378" s="0" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="E378" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F378" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B379" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C379" s="0" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="D379" s="0" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="E379" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F379" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B380" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C380" s="0" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="D380" s="0" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="E380" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F380" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B381" s="0" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="C381" s="0" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="D381" s="0" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="E381" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F381" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B382" s="0" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="C382" s="0" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="D382" s="0" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="E382" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F382" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B383" s="0" t="s">
-        <v>452</v>
+        <v>288</v>
       </c>
       <c r="C383" s="0" t="s">
-        <v>298</v>
+        <v>458</v>
       </c>
       <c r="D383" s="0" t="s">
-        <v>299</v>
+        <v>459</v>
       </c>
       <c r="E383" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F383" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B384" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C384" s="0" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="D384" s="0" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="E384" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F384" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B385" s="0" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C385" s="0" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="D385" s="0" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="E385" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F385" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B386" s="0" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
       <c r="C386" s="0" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="D386" s="0" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="E386" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F386" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B387" s="0" t="s">
-        <v>305</v>
+        <v>466</v>
       </c>
       <c r="C387" s="0" t="s">
-        <v>459</v>
+        <v>313</v>
       </c>
       <c r="D387" s="0" t="s">
-        <v>460</v>
+        <v>314</v>
       </c>
       <c r="E387" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F387" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B388" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C388" s="0" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="D388" s="0" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="E388" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F388" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B389" s="0" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
       <c r="C389" s="0" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="D389" s="0" t="s">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="E389" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F389" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B390" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C390" s="0" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="D390" s="0" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="E390" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F390" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B391" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C391" s="0" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="D391" s="0" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="E391" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F391" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B392" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C392" s="0" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="D392" s="0" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="E392" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F392" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B393" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C393" s="0" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="D393" s="0" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="E393" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F393" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B394" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C394" s="0" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="D394" s="0" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="E394" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F394" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B395" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C395" s="0" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="D395" s="0" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="E395" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F395" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B396" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C396" s="0" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="D396" s="0" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="E396" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F396" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B397" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C397" s="0" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="D397" s="0" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="E397" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F397" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="0" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B398" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C398" s="0" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="D398" s="0" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="E398" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F398" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A399" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="B399" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="C399" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="D399" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="E399" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F399" s="0" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="0" t="s">
-        <v>483</v>
+        <v>326</v>
       </c>
       <c r="B400" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C400" s="0" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
       <c r="D400" s="0" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c r="E400" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F400" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="0" t="s">
-        <v>483</v>
+        <v>326</v>
       </c>
       <c r="B401" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C401" s="0" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="D401" s="0" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="E401" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F401" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="0" t="s">
-        <v>483</v>
+        <v>326</v>
       </c>
       <c r="B402" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C402" s="0" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="D402" s="0" t="s">
-        <v>426</v>
+        <v>496</v>
       </c>
       <c r="E402" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F402" s="0" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A403" s="0" t="s">
-        <v>483</v>
-      </c>
-      <c r="B403" s="0" t="s">
-        <v>305</v>
-      </c>
-      <c r="C403" s="0" t="s">
-        <v>488</v>
-      </c>
-      <c r="D403" s="0" t="s">
-        <v>489</v>
-      </c>
-      <c r="E403" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="F403" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="0" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="B404" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C404" s="0" t="s">
-        <v>459</v>
+        <v>498</v>
       </c>
       <c r="D404" s="0" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
       <c r="E404" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F404" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A405" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="B405" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="C405" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="D405" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="E405" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F405" s="0" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="0" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="B406" s="0" t="s">
-        <v>492</v>
+        <v>288</v>
       </c>
       <c r="C406" s="0" t="s">
-        <v>298</v>
+        <v>439</v>
       </c>
       <c r="D406" s="0" t="s">
-        <v>299</v>
+        <v>440</v>
       </c>
       <c r="E406" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F406" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A407" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="B407" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="C407" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="D407" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="E407" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F407" s="0" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="0" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="B408" s="0" t="s">
-        <v>494</v>
+        <v>288</v>
       </c>
       <c r="C408" s="0" t="s">
-        <v>295</v>
+        <v>473</v>
       </c>
       <c r="D408" s="0" t="s">
-        <v>328</v>
+        <v>504</v>
       </c>
       <c r="E408" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F408" s="0" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A409" s="0" t="s">
-        <v>493</v>
-      </c>
-      <c r="B409" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="C409" s="0" t="s">
-        <v>384</v>
-      </c>
-      <c r="D409" s="0" t="s">
-        <v>385</v>
-      </c>
-      <c r="E409" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="F409" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="0" t="s">
-        <v>493</v>
+        <v>505</v>
       </c>
       <c r="B410" s="0" t="s">
-        <v>494</v>
+        <v>506</v>
       </c>
       <c r="C410" s="0" t="s">
-        <v>386</v>
+        <v>313</v>
       </c>
       <c r="D410" s="0" t="s">
-        <v>387</v>
+        <v>314</v>
       </c>
       <c r="E410" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F410" s="0" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A411" s="0" t="s">
-        <v>493</v>
-      </c>
-      <c r="B411" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="C411" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="D411" s="0" t="s">
-        <v>496</v>
-      </c>
-      <c r="E411" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="F411" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="0" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="B412" s="0" t="s">
-        <v>494</v>
+        <v>508</v>
       </c>
       <c r="C412" s="0" t="s">
-        <v>497</v>
+        <v>310</v>
       </c>
       <c r="D412" s="0" t="s">
-        <v>498</v>
+        <v>342</v>
       </c>
       <c r="E412" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F412" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="0" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="B413" s="0" t="s">
-        <v>494</v>
+        <v>508</v>
       </c>
       <c r="C413" s="0" t="s">
-        <v>289</v>
+        <v>398</v>
       </c>
       <c r="D413" s="0" t="s">
-        <v>422</v>
+        <v>399</v>
       </c>
       <c r="E413" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F413" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="0" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="B414" s="0" t="s">
-        <v>494</v>
+        <v>508</v>
       </c>
       <c r="C414" s="0" t="s">
-        <v>448</v>
+        <v>400</v>
       </c>
       <c r="D414" s="0" t="s">
-        <v>449</v>
+        <v>401</v>
       </c>
       <c r="E414" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F414" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A415" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="B415" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="C415" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="D415" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="E415" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F415" s="0" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="0" t="s">
-        <v>312</v>
+        <v>507</v>
       </c>
       <c r="B416" s="0" t="s">
-        <v>305</v>
+        <v>508</v>
       </c>
       <c r="C416" s="0" t="s">
-        <v>499</v>
+        <v>511</v>
       </c>
       <c r="D416" s="0" t="s">
-        <v>500</v>
+        <v>512</v>
       </c>
       <c r="E416" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F416" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="0" t="s">
-        <v>312</v>
+        <v>507</v>
       </c>
       <c r="B417" s="0" t="s">
-        <v>305</v>
+        <v>508</v>
       </c>
       <c r="C417" s="0" t="s">
-        <v>501</v>
+        <v>304</v>
       </c>
       <c r="D417" s="0" t="s">
-        <v>502</v>
+        <v>436</v>
       </c>
       <c r="E417" s="0" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F417" s="0" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A419" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="B419" s="0" t="s">
-        <v>305</v>
-      </c>
-      <c r="C419" s="0" t="s">
-        <v>503</v>
-      </c>
-      <c r="D419" s="0" t="s">
-        <v>504</v>
-      </c>
-      <c r="E419" s="0" t="s">
-        <v>505</v>
-      </c>
-      <c r="F419" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="H419" s="0" t="s">
-        <v>506</v>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A418" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="B418" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="C418" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="D418" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="E418" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F418" s="0" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="0" t="s">
-        <v>287</v>
+        <v>326</v>
       </c>
       <c r="B420" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C420" s="0" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="D420" s="0" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="E420" s="0" t="s">
-        <v>505</v>
+        <v>306</v>
       </c>
       <c r="F420" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="H420" s="0" t="s">
-        <v>509</v>
+        <v>307</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="0" t="s">
-        <v>287</v>
+        <v>326</v>
       </c>
       <c r="B421" s="0" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="C421" s="0" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="D421" s="0" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="E421" s="0" t="s">
-        <v>505</v>
+        <v>306</v>
       </c>
       <c r="F421" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="H421" s="0" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A422" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="B422" s="0" t="s">
-        <v>513</v>
-      </c>
-      <c r="C422" s="0" t="s">
-        <v>514</v>
-      </c>
-      <c r="D422" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="E422" s="0" t="s">
-        <v>505</v>
-      </c>
-      <c r="F422" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="0" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="B423" s="0" t="s">
-        <v>513</v>
+        <v>288</v>
       </c>
       <c r="C423" s="0" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D423" s="0" t="s">
-        <v>294</v>
+        <v>518</v>
       </c>
       <c r="E423" s="0" t="s">
-        <v>505</v>
+        <v>519</v>
       </c>
       <c r="F423" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
+      </c>
+      <c r="H423" s="0" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="0" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="B424" s="0" t="s">
-        <v>516</v>
+        <v>288</v>
       </c>
       <c r="C424" s="0" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="D424" s="0" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="E424" s="0" t="s">
-        <v>505</v>
+        <v>519</v>
       </c>
       <c r="F424" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="H424" s="0" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="0" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="B425" s="0" t="s">
-        <v>520</v>
+        <v>288</v>
       </c>
       <c r="C425" s="0" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="D425" s="0" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="E425" s="0" t="s">
-        <v>505</v>
+        <v>519</v>
       </c>
       <c r="F425" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="H425" s="0" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="0" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="B426" s="0" t="s">
-        <v>513</v>
+        <v>527</v>
       </c>
       <c r="C426" s="0" t="s">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="D426" s="0" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="E426" s="0" t="s">
-        <v>505</v>
+        <v>519</v>
       </c>
       <c r="F426" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="0" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="B427" s="0" t="s">
-        <v>516</v>
+        <v>527</v>
       </c>
       <c r="C427" s="0" t="s">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c r="D427" s="0" t="s">
-        <v>524</v>
+        <v>309</v>
       </c>
       <c r="E427" s="0" t="s">
-        <v>505</v>
+        <v>519</v>
       </c>
       <c r="F427" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="H427" s="0" t="s">
-        <v>524</v>
+        <v>307</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="0" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="B428" s="0" t="s">
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="C428" s="0" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="D428" s="0" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
       <c r="E428" s="0" t="s">
-        <v>505</v>
+        <v>519</v>
       </c>
       <c r="F428" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="H428" s="0" t="s">
-        <v>524</v>
+        <v>533</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="0" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="B429" s="0" t="s">
-        <v>513</v>
+        <v>534</v>
       </c>
       <c r="C429" s="0" t="s">
-        <v>526</v>
+        <v>535</v>
       </c>
       <c r="D429" s="0" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
       <c r="E429" s="0" t="s">
-        <v>505</v>
+        <v>519</v>
       </c>
       <c r="F429" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
+      </c>
+      <c r="H429" s="0" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="0" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="B430" s="0" t="s">
-        <v>516</v>
+        <v>527</v>
       </c>
       <c r="C430" s="0" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
       <c r="D430" s="0" t="s">
-        <v>529</v>
+        <v>311</v>
       </c>
       <c r="E430" s="0" t="s">
-        <v>505</v>
+        <v>519</v>
       </c>
       <c r="F430" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="H430" s="0" t="s">
-        <v>530</v>
+        <v>307</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="0" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="B431" s="0" t="s">
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="C431" s="0" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="D431" s="0" t="s">
-        <v>529</v>
+        <v>538</v>
       </c>
       <c r="E431" s="0" t="s">
-        <v>505</v>
+        <v>519</v>
       </c>
       <c r="F431" s="0" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="H431" s="0" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A432" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B432" s="0" t="s">
+        <v>534</v>
+      </c>
+      <c r="C432" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="D432" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="E432" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="F432" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="H432" s="0" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A433" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B433" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="C433" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="D433" s="0" t="s">
+        <v>541</v>
+      </c>
+      <c r="E433" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="F433" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A434" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B434" s="0" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C434" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="D434" s="0" t="s">
+        <v>543</v>
+      </c>
+      <c r="E434" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="F434" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="H434" s="0" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A435" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B435" s="0" t="s">
+        <v>534</v>
+      </c>
+      <c r="C435" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="D435" s="0" t="s">
+        <v>543</v>
+      </c>
+      <c r="E435" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="F435" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="H435" s="0" t="s">
+        <v>544</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update comment in basic identified missing file: shaconemo revision r193 ==> r199
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">agessc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in one of the shaconemo (r193) ping files. </t>
+    <t xml:space="preserve">Identified in one of the shaconemo (199) ping files. </t>
   </si>
   <si>
     <t xml:space="preserve">Thomas Reerink</t>
@@ -1777,8 +1777,8 @@
   </sheetPr>
   <dimension ref="A1:H435"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A279" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A298" activeCellId="0" sqref="298:298"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A370" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A298" activeCellId="1" sqref="E3:E255 A298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Update the lists of identified-missing and ignored vars for the updates in the pre files
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -82,7 +82,7 @@
     <t>Mole Concentration of CFC-11 in sea water</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in one of the shaconemo (212) ping files. </t>
+    <t xml:space="preserve">Identified in one of the shaconemo (216) ping files. </t>
   </si>
   <si>
     <t>Thomas Reerink</t>
@@ -1291,7 +1291,7 @@
     <t>phyfeos</t>
   </si>
   <si>
-    <t>Surface Mass Concentration of Diazotrophs expressed as Chlorophyll in sea water</t>
+    <t>Surface Mole Concentration of Total Phytoplankton expressed as Iron in Sea Water</t>
   </si>
   <si>
     <t>hfbasinpmadv</t>

</xml_diff>

<commit_message>
Update for last Shaconemo revision - same variables as previously this time
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -193,7 +193,7 @@
     <t xml:space="preserve">Sea Surface Total Chlorophyll Mass Concentration</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in one of the shaconemo (238) ping files. </t>
+    <t xml:space="preserve">Identified in one of the shaconemo (239) ping files. </t>
   </si>
   <si>
     <t xml:space="preserve">Thomas Reerink</t>
@@ -5717,8 +5717,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A652" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A668" activeCellId="0" sqref="A668"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="22" sqref="G14:G16 G20:G57 G122:G127 G129:G160 G162:G191 G207:G208 G210:G223 G225:G249 G251:G253 G255:G259 G261 G266:G325 G329 G331 G351:G353 G486:G497 G499:G504 G512 G599 G601:G613 G617 G655:G657 G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5731,7 +5731,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="200.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="200.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.67"/>
   </cols>

</xml_diff>

<commit_message>
Add again manually the IyrGre ISMIP6 (step 3) variables modelCellAreai, sftgif and sftgrf to the basic identified file, this add has been done in a commit at 24 april 2018, but somewhere got lost.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3570" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3600" uniqueCount="1108">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -3317,6 +3317,33 @@
   </si>
   <si>
     <t xml:space="preserve">Available in LPJ-GUESS.  Already exist as - evspsblveg - Total Evaporation of intercepted water from Canopy [kg m-2 s-1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IyrGre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modelCellAreai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cell area of the ice sheet model.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PISM model probably uses a constant and uniform grid size within EC-Earth, this grid size can be reported or a filed from the grid sizes can be provided in a post processing phase.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal area of ice-sheet grid cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xgre ygre time typeli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xgre ygre time typegis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Greenland this is the same as sftgif. We do not have an Antarctic ice sheet.</t>
   </si>
 </sst>
 </file>
@@ -3428,8 +3455,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A362" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A377" activeCellId="0" sqref="377:382"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A366" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A388" activeCellId="0" sqref="A388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3443,7 +3470,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
@@ -16298,6 +16325,116 @@
         <v>27</v>
       </c>
     </row>
+    <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A385" s="0" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B385" s="0" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C385" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D385" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E385" s="0" t="s">
+        <v>1101</v>
+      </c>
+      <c r="F385" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="G385" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H385" s="0" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I385" s="0" t="s">
+        <v>1103</v>
+      </c>
+      <c r="J385" s="0" t="s">
+        <v>1104</v>
+      </c>
+      <c r="K385" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A386" s="0" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B386" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C386" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D386" s="0" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E386" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="F386" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G386" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H386" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="I386" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J386" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="K386" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A387" s="0" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B387" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C387" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D387" s="0" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E387" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F387" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G387" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H387" s="0" t="s">
+        <v>1107</v>
+      </c>
+      <c r="I387" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J387" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K387" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Recompile the ignored & identified missing lists: the second part of the manual additons #290.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="356">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -1061,6 +1061,33 @@
   </si>
   <si>
     <t xml:space="preserve">The  downward northward stress associated with the models parameterization of the planetary boundary layer. (This request is related to a WGNE effort to understand how models parameterize the surface stresses.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IyrGre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modelCellAreai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cell area of the ice sheet model.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PISM model probably uses a constant and uniform grid size within EC-Earth, this grid size can be reported or a filed from the grid sizes can be provided in a post processing phase.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal area of ice-sheet grid cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xgre ygre time typeli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xgre ygre time typegis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Greenland this is the same as sftgif. We do not have an Antarctic ice sheet.</t>
   </si>
 </sst>
 </file>
@@ -1144,12 +1171,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1170,10 +1201,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K96"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A87" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A98" activeCellId="0" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4035,6 +4066,158 @@
         <v>342</v>
       </c>
     </row>
+    <row r="101" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G101" s="2" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917e2ba-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="F104" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="G104" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/865d0e00-53e6-11e6-b524-5404a60d96b5.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="J104" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="K104" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="E105" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="F105" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G105" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J105" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="K105" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="E106" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F106" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G106" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J106" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K106" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Correct identification of expn expp see issue at ec-earth portal 518-146. #314.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -667,25 +667,25 @@
     <t xml:space="preserve">Sinking Particulate Organic Nitrogen Flux</t>
   </si>
   <si>
+    <t xml:space="preserve">Available in PISCES: EXPC * (16/122). Not available inLPJ-GUESS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Warlind, Raffaele Bernardello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In accordance with common usage in geophysical disciplines, 'flux' implies per unit area, called 'flux density' in physics.   'Sinking' is the gravitational settling of particulate matter suspended in a liquid. A sinking flux is positive downwards and is calculated relative to the movement of the surrounding fluid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,CMIP,GeoMIP,LUMIP,OMIP,VIACSAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinking Particulate Organic Phosphorus Flux</t>
+  </si>
+  <si>
     <t xml:space="preserve">Available in PISCES: EXPC * (1/122). Not available inLPJ-GUESS.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David Warlind, Raffaele Bernardello</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In accordance with common usage in geophysical disciplines, 'flux' implies per unit area, called 'flux density' in physics.   'Sinking' is the gravitational settling of particulate matter suspended in a liquid. A sinking flux is positive downwards and is calculated relative to the movement of the surrounding fluid.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AerChemMIP,CMIP,GeoMIP,LUMIP,OMIP,VIACSAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sinking Particulate Organic Phosphorus Flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available in PISCES: EXPC * (16/122). Not available inLPJ-GUESS.</t>
   </si>
   <si>
     <t xml:space="preserve">AERmon</t>
@@ -1203,8 +1203,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A87" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A98" activeCellId="0" sqref="A98"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E50" activeCellId="0" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1218,7 +1218,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>

</xml_diff>

<commit_message>
Create the ignore and identified missing list from the pre lists, including the manual edits as described in update-basic-identifiedmissing-ignored-files.sh. In this case #385 & #389 are taken for the first time. Also #381 and the fix #387 are addressed.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="256">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -274,7 +274,7 @@
     <t xml:space="preserve">Tendency of Air Temperature Due to Radiative Heating</t>
   </si>
   <si>
-    <t xml:space="preserve">Available in IFS: T-tendency from radiation: grib 128.95</t>
+    <t xml:space="preserve">grib 126.95                                                                Available in IFS: T-tendency from radiation: grib 128.95</t>
   </si>
   <si>
     <t xml:space="preserve">Tendency of Air Temperature due to Radiative Heating</t>
@@ -289,7 +289,7 @@
     <t xml:space="preserve">s-1</t>
   </si>
   <si>
-    <t xml:space="preserve">Adding all the q-tendencies, thus: grib 128.94 + 128.99 + 128.106 + 128.110.  Alternatively, in IFS: just estimating the delta q per month. So far no direct grib code for the totoal q-tendency found</t>
+    <t xml:space="preserve">Grib 126.94 + 126.99 + 126.106 + 126.110  Adding all the q-tendencies, thus: grib 128.94 + 128.99 + 128.106 + 128.110.  Alternatively, in IFS: just estimating the delta q per month. So far no direct grib code for the totoal q-tendency found</t>
   </si>
   <si>
     <t xml:space="preserve">tnhusc</t>
@@ -298,7 +298,7 @@
     <t xml:space="preserve">Tendency of Specific Humidity Due to Convection</t>
   </si>
   <si>
-    <t xml:space="preserve">Available in IFS: q-tendency from convection: grib 128.106</t>
+    <t xml:space="preserve">grib 126.106                                                              Available in IFS: q-tendency from convection: grib 128.106</t>
   </si>
   <si>
     <t xml:space="preserve">tnhusmp</t>
@@ -307,7 +307,7 @@
     <t xml:space="preserve">Tendency of Specific Humidity Due to Model Physics</t>
   </si>
   <si>
-    <t xml:space="preserve">Adding all the q-tendencies without advection, thus: grib 128.99 + 128.106 + 128.110.</t>
+    <t xml:space="preserve">grib 126.99 + 126.106 + 126.110                      Adding all the q-tendencies without advection, thus: grib 128.99 + 128.106 + 128.110.</t>
   </si>
   <si>
     <t xml:space="preserve">Tendency of specific humidity due to model physics. This includes sources and sinks from parametrized moist physics (e.g. convection, boundary layer, stratiform condensation/evaporation, etc.) and excludes sources and sinks from resolved dynamics or from horizontal or vertical numerical diffusion not associated with model physics.  For example any diffusive mixing by the boundary layer scheme would be included.</t>
@@ -319,7 +319,7 @@
     <t xml:space="preserve">ISCCP Total Cloud Cover Percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP: ISCCP total cloud area, CVEXTRA(5)='94 ISCCP_TOTALCLDAREA'</t>
+    <t xml:space="preserve">COSP grib 126.44   CVEXTR2(5)='ISCCP_TOTALCLD'</t>
   </si>
   <si>
     <t xml:space="preserve">Klaus</t>
@@ -337,7 +337,7 @@
     <t xml:space="preserve">ISCCP Mean Cloud Albedo</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP: ISCCP cloud albedo, CVEXTRA(7)='96 ISCCP_MEANALBEDOCLD'</t>
+    <t xml:space="preserve">COSP grib 126.46   CVEXTR2(7)='ISCCP_MEANALBCLD'</t>
   </si>
   <si>
     <t xml:space="preserve">ISCCP Mean Cloud Albedo. Time-means are weighted by the ISCCP Total Cloud Fraction {:cltisccp} - see  http://cfmip.metoffice.com/COSP.html</t>
@@ -355,7 +355,7 @@
     <t xml:space="preserve">Pa</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP: ISCCP cloud top pressure, CVEXTRA(6)='95 ISCCP_MEANPTOP'</t>
+    <t xml:space="preserve">COSP grib 126.45   CVEXTR2(6)='ISCCP_MEANPTOP'</t>
   </si>
   <si>
     <t xml:space="preserve">ISCCP Mean Cloud Top Pressure. Time-means are weighted by the ISCCP Total Cloud Fraction {:cltisccp} - see  http://cfmip.metoffice.com/COSP.html</t>
@@ -367,7 +367,7 @@
     <t xml:space="preserve">CALIPSO Total Cloud Cover Percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP: CALIPSO total cloud cover, CVEXTRA(4)='93 CALIPSO_CLDLAYER TOTAL'</t>
+    <t xml:space="preserve">COSP grib 126.43   CVEXTR2(4)='CALIPSO_TCC'</t>
   </si>
   <si>
     <t xml:space="preserve">'X_area_fraction' means the fraction of horizontal area occupied by X. 'X_area' means the horizontal area occupied by X within the grid cell. Cloud area fraction is also called 'cloud amount' and 'cloud cover'. The cloud area fraction is for the whole atmosphere column, as seen from the surface or the top of the atmosphere. The cloud area fraction in a layer of the atmosphere has the standard name cloud_area_fraction_in_atmosphere_layer.</t>
@@ -385,7 +385,7 @@
     <t xml:space="preserve">CALIPSO Low Level Cloud Cover Percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP: CALIPSO low cloud cover, CVEXTRA(1)='90 CALIPSO_CLDLAYER LOW'</t>
+    <t xml:space="preserve">COSP grib 126.40   CVEXTR2(1)='CALIPSO_LCC'</t>
   </si>
   <si>
     <t xml:space="preserve">Percentage cloud cover in layer centred on 840hPa</t>
@@ -400,7 +400,7 @@
     <t xml:space="preserve">CALIPSO Mid Level Cloud Cover Percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP: CALIPSO mid cloud cover, CVEXTRA(2)='91 CALIPSO_CLDLAYER MID'</t>
+    <t xml:space="preserve">COSP grib 126.41   CVEXTR2(2)='CALIPSO_MCC'</t>
   </si>
   <si>
     <t xml:space="preserve">Percentage cloud cover in layer centred on 560hPa</t>
@@ -415,7 +415,7 @@
     <t xml:space="preserve">CALIPSO High Level Cloud Area Percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP: CALIPSO high cloud cover, CVEXTRA(3)='92 CALIPSO_CLDLAYER HIGH'</t>
+    <t xml:space="preserve">COSP grib 126.42   CVEXTR2(3)='CALIPSO_HCC'</t>
   </si>
   <si>
     <t xml:space="preserve">Percentage cloud cover in layer centred on 220hPa</t>
@@ -466,19 +466,64 @@
     <t xml:space="preserve">Runoff flux over land ice is the difference between any available liquid water in the snowpack less any refreezing. Computed as the sum of rainfall and melt of snow or ice less any refreezing or water retained in the snowpack</t>
   </si>
   <si>
+    <t xml:space="preserve">Omon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfibthermds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude olevel time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Flux into Sea Water Due to Iceberg Thermodynamics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W m-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in OPA: &lt;field id="hflx_cal_cea"  long_name="heat flux due to calving"   standard_name="heat_flux_into_sea_water_due_to_iceberg_thermodynamics   &lt;!-- available if key_oasis3 + conservative method --&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In accordance with common usage in geophysical disciplines, 'flux' implies per unit area, called 'flux density' in physics.  The specification of a physical process by the phrase due_to_process means that the quantity named is a  single term in a sum of terms which together compose the general quantity  named by omitting the phrase.  ' Iceberg thermodynamics' refers to the addition or subtraction of mass due to surface and basal fluxes, i.e., due to melting, sublimation and fusion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,C4MIP,CMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,OMIP,VolMIP</t>
+  </si>
+  <si>
     <t xml:space="preserve">AERmon</t>
   </si>
   <si>
+    <t xml:space="preserve">cdnc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Liquid Droplet Number Concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grib 126.20 / 126.22  in namelist.ifs.cloudact+diag.sh  CVEXTRA(1)='CDNC' which is a PEXTRA variable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Droplet Number Concentration in liquid water clouds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,CFMIP,DAMIP</t>
+  </si>
+  <si>
     <t xml:space="preserve">rlutaf</t>
   </si>
   <si>
     <t xml:space="preserve">TOA Outgoing Aerosol-Free Longwave Radiation</t>
   </si>
   <si>
-    <t xml:space="preserve">W m-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available from double radiation call in IFS. See also PEXTRA issue #403</t>
+    <t xml:space="preserve">grib 126.73                      Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
   </si>
   <si>
     <t xml:space="preserve">Flux corresponding to rlut resulting from aerosol-free call to radiation, following Ghan (ACP, 2013)</t>
@@ -493,7 +538,7 @@
     <t xml:space="preserve">TOA Outgoing Clear-Sky, Aerosol-Free Longwave Radiation</t>
   </si>
   <si>
-    <t xml:space="preserve">Available from double radiation call in IFS. See also PEXTRA issue #404</t>
+    <t xml:space="preserve">grib 126.72                       Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
   </si>
   <si>
     <t xml:space="preserve">Flux corresponding to rlutcs resulting from aerosol-free call to radiation, following Ghan (ACP, 2013)</t>
@@ -505,7 +550,7 @@
     <t xml:space="preserve">TOA Outgoing Aerosol-Free Shortwave Radiation</t>
   </si>
   <si>
-    <t xml:space="preserve">Available from double radiation call in IFS. See also PEXTRA issue #403   aerosol free</t>
+    <t xml:space="preserve">grib 128.212-126.069  Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
   </si>
   <si>
     <t xml:space="preserve">Flux corresponding to rsut resulting from aerosol-free call to radiation, following Ghan (ACP, 2013)</t>
@@ -515,39 +560,6 @@
   </si>
   <si>
     <t xml:space="preserve">Emon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conccn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aerosol Number Concentration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available in TM5, though yet to be added by Tommi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tommi Bergman, Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'Number concentration' means the number of particles or other specified objects per unit volume. 'Aerosol' means the system of suspended liquid or solid particles in air (except cloud droplets) and their carrier gas, the air itself. 'Ambient_aerosol' means that the aerosol is measured or modelled at the ambient state of pressure, temperature and relative humidity that exists in its immediate environment. 'Ambient aerosol particles' are aerosol particles that have taken up ambient water through hygroscopic growth. The extent of hygroscopic growth depends on the relative humidity and the composition of the particles.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GeoMIP,VIACSAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sconcss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Concentration of Sea-Salt Aerosol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg m-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mass concentration of sea-salt dry aerosol in air in model lowest layer</t>
   </si>
   <si>
     <t xml:space="preserve">uqint</t>
@@ -891,8 +903,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A69" activeCellId="0" sqref="69:78"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1890,73 +1902,37 @@
         <v>149</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>13</v>
+        <v>150</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>70</v>
+        <v>151</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G35" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a640b0-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bd938fec017c18d3eee106db55f924c5.html","web")</f>
         <v>0</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>65</v>
+        <v>155</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="G36" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a673b4-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="0" t="s">
         <v>157</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="J36" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="K36" s="0" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>159</v>
@@ -1965,73 +1941,109 @@
         <v>13</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>160</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="G37" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a56fd2-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cfe4bddb7dbbfc57c19837e7f99d2dda.html","web")</f>
         <v>0</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I37" s="0" t="s">
         <v>65</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a640b0-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="G39" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/70b0b8239a6ffb48b4a4f3086da12150.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a673b4-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
         <v>0</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="I39" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="K39" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="J39" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="K39" s="0" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>13</v>
@@ -2040,70 +2052,34 @@
         <v>70</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="G40" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/31a3caf70db7a8ed71e8d0a226365105.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a56fd2-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
         <v>0</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>169</v>
+        <v>65</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="K40" s="0" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="F41" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="G41" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H41" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="I41" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="J41" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="K41" s="0" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>13</v>
@@ -2112,31 +2088,31 @@
         <v>70</v>
       </c>
       <c r="E42" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="0" t="s">
         <v>183</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="G42" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H42" s="0" t="s">
-        <v>184</v>
       </c>
       <c r="I42" s="0" t="s">
         <v>57</v>
       </c>
       <c r="J42" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="K42" s="0" t="s">
         <v>185</v>
-      </c>
-      <c r="K42" s="0" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>186</v>
@@ -2151,31 +2127,31 @@
         <v>187</v>
       </c>
       <c r="F43" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="0" t="s">
         <v>188</v>
-      </c>
-      <c r="G43" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H43" s="0" t="s">
-        <v>189</v>
       </c>
       <c r="I43" s="0" t="s">
         <v>57</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>13</v>
@@ -2184,31 +2160,31 @@
         <v>70</v>
       </c>
       <c r="E44" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="0" t="s">
         <v>193</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="G44" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H44" s="0" t="s">
-        <v>194</v>
       </c>
       <c r="I44" s="0" t="s">
         <v>57</v>
       </c>
       <c r="J44" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="K44" s="0" t="s">
         <v>195</v>
-      </c>
-      <c r="K44" s="0" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>196</v>
@@ -2223,31 +2199,31 @@
         <v>197</v>
       </c>
       <c r="F45" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H45" s="0" t="s">
         <v>198</v>
-      </c>
-      <c r="G45" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>199</v>
       </c>
       <c r="I45" s="0" t="s">
         <v>57</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K45" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>13</v>
@@ -2256,13 +2232,13 @@
         <v>70</v>
       </c>
       <c r="E46" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="F46" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="F46" s="0" t="s">
-        <v>198</v>
-      </c>
       <c r="G46" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H46" s="0" t="s">
@@ -2275,12 +2251,12 @@
         <v>204</v>
       </c>
       <c r="K46" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>205</v>
@@ -2289,73 +2265,73 @@
         <v>13</v>
       </c>
       <c r="D47" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E47" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="F47" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="F47" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G47" s="0" t="n">
+      <c r="I47" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="K47" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
-      <c r="H47" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="I47" s="0" t="s">
+      <c r="H48" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="I48" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="J47" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="K47" s="0" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G49" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H49" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="I49" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="J49" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="K49" s="0" t="s">
-        <v>212</v>
+      <c r="J48" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="K48" s="0" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>13</v>
@@ -2364,34 +2340,34 @@
         <v>70</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G50" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
         <v>0</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="I50" s="0" t="s">
         <v>100</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K50" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>13</v>
@@ -2400,34 +2376,34 @@
         <v>70</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="G51" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
         <v>0</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="I51" s="0" t="s">
         <v>100</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K51" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>13</v>
@@ -2436,427 +2412,427 @@
         <v>70</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="G52" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
         <v>0</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I52" s="0" t="s">
         <v>100</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="K52" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G53" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
         <v>0</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I53" s="0" t="s">
         <v>100</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="K53" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F54" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G54" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
         <v>0</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="I54" s="0" t="s">
         <v>100</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="K54" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G55" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
         <v>0</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I55" s="0" t="s">
         <v>100</v>
       </c>
       <c r="J55" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="K55" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="J56" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="K55" s="0" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="F57" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G57" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H57" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="I57" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="J57" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="K57" s="0" t="s">
-        <v>215</v>
+      <c r="K56" s="0" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F58" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G58" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
         <v>0</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I58" s="0" t="s">
         <v>100</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="K58" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F59" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G59" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
         <v>0</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="I59" s="0" t="s">
         <v>100</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="K59" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F60" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G60" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
         <v>0</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I60" s="0" t="s">
         <v>100</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K60" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B61" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H61" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="I61" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="J61" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="K61" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="C61" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="F61" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="G61" s="0" t="n">
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="G62" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
-      <c r="H61" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="I61" s="0" t="s">
+      <c r="H62" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="I62" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="J61" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="K61" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="B63" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="D63" s="0" t="s">
+      <c r="J62" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E63" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="F63" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G63" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H63" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I63" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J63" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="K63" s="0" t="s">
-        <v>181</v>
+      <c r="K62" s="0" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="G64" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
         <v>0</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="I64" s="0" t="s">
         <v>80</v>
       </c>
       <c r="J64" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="K64" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="E65" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="K64" s="0" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="F66" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G66" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H66" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="I66" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J66" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="K66" s="0" t="s">
-        <v>140</v>
+      <c r="F65" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G65" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H65" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="K65" s="0" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>233</v>
@@ -2865,37 +2841,37 @@
         <v>13</v>
       </c>
       <c r="D67" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E67" s="0" t="s">
         <v>234</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>235</v>
       </c>
       <c r="F67" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G67" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I67" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K67" s="0" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>12</v>
+        <v>237</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>13</v>
@@ -2904,175 +2880,211 @@
         <v>238</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>15</v>
+        <v>239</v>
       </c>
       <c r="F68" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G68" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
         <v>0</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>17</v>
+        <v>240</v>
       </c>
       <c r="I68" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J68" s="0" t="s">
-        <v>19</v>
+        <v>241</v>
       </c>
       <c r="K68" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H69" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I69" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K69" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B73" s="2" t="s">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73" s="2" t="s">
+      <c r="C74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="F73" s="2" t="s">
+      <c r="E74" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G73" s="2" t="str">
+      <c r="G74" s="2" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917e2ba-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H73" s="2" t="s">
+      <c r="H74" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I73" s="2" t="s">
+      <c r="I74" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J73" s="2" t="s">
+      <c r="J74" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="K73" s="2" t="s">
+      <c r="K74" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="B76" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D76" s="0" t="s">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="E76" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="F76" s="0" t="s">
+      <c r="E77" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="F77" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="G76" s="0" t="str">
+      <c r="G77" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/865d0e00-53e6-11e6-b524-5404a60d96b5.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H76" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="I76" s="2" t="s">
+      <c r="H77" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="J77" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="K77" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="J76" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="K76" s="0" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="E77" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="F77" s="0" t="s">
+      <c r="B78" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="F78" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G77" s="0" t="str">
+      <c r="G78" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H77" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="I77" s="2" t="s">
+      <c r="H78" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="I78" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="J77" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="K77" s="0" t="s">
+      <c r="J78" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="K78" s="0" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="B78" s="0" t="s">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B79" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C78" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="E78" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="F78" s="0" t="s">
+      <c r="C79" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="F79" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G78" s="0" t="str">
+      <c r="G79" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H78" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I78" s="2" t="s">
+      <c r="H79" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="I79" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="J78" s="0" t="s">
+      <c r="J79" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="K78" s="0" t="s">
+      <c r="K79" s="0" t="s">
         <v>140</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Move CFmon tnt from identified missing to ignored list, as we cannot more provide then a delta field, which anyone can do #143.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="244">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -250,34 +250,25 @@
     <t xml:space="preserve">CFmon</t>
   </si>
   <si>
-    <t xml:space="preserve">tnt</t>
+    <t xml:space="preserve">tntr</t>
   </si>
   <si>
     <t xml:space="preserve">longitude latitude alevel time</t>
   </si>
   <si>
-    <t xml:space="preserve">Tendency of Air Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alternatively, just estimating the delta T per month. No direct grib code for the totoal T-tendency found. In IFS from Cycle 39R1: add all the T-Tendencies: grib 128.93 + 128.95 + 128.98 + 128.102 + 128.105 + 128.109. But with IFS cycle 36 the T-tendency of gravity wave drag grib 128.102 is bugged until Cycle 39R1. This has been checked by Gijs with ECMWF: https://software.ecmwf.int/wiki/pages/viewpage.action?pageId=97384581</t>
+    <t xml:space="preserve">Tendency of Air Temperature Due to Radiative Heating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.95                                                                Available in IFS: T-tendency from radiation: grib 128.95</t>
   </si>
   <si>
     <t xml:space="preserve">Twan, Thomas &amp; Gijs</t>
   </si>
   <si>
+    <t xml:space="preserve">Tendency of Air Temperature due to Radiative Heating</t>
+  </si>
+  <si>
     <t xml:space="preserve">AerChemMIP,CFMIP,DAMIP,GeoMIP,HighResMIP,PMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tntr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tendency of Air Temperature Due to Radiative Heating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grib 126.95                                                                Available in IFS: T-tendency from radiation: grib 128.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tendency of Air Temperature due to Radiative Heating</t>
   </si>
   <si>
     <t xml:space="preserve">tnhus</t>
@@ -876,8 +867,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -891,7 +882,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
@@ -1347,7 +1338,7 @@
         <v>63</v>
       </c>
       <c r="G17" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/93a0ba1f23bfc41b720ea68951d28144.html","web")</f>
         <v>0</v>
       </c>
       <c r="H17" s="0" t="s">
@@ -1357,10 +1348,10 @@
         <v>80</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1368,7 +1359,7 @@
         <v>75</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>13</v>
@@ -1377,26 +1368,26 @@
         <v>77</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>63</v>
       </c>
       <c r="G18" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/93a0ba1f23bfc41b720ea68951d28144.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/52f043533a691ca5721460e316c3a328.html","web")</f>
         <v>0</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1404,7 +1395,7 @@
         <v>75</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>13</v>
@@ -1413,26 +1404,26 @@
         <v>77</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="G19" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/52f043533a691ca5721460e316c3a328.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
         <v>0</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1440,7 +1431,7 @@
         <v>75</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>13</v>
@@ -1449,13 +1440,13 @@
         <v>77</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G20" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d576b3fc447c37d782926441428ffd.html","web")</f>
         <v>0</v>
       </c>
       <c r="H20" s="0" t="s">
@@ -1465,10 +1456,10 @@
         <v>80</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1488,10 +1479,10 @@
         <v>91</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G21" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d576b3fc447c37d782926441428ffd.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6e30ba1e2c19dcbd85faa176d4eae596.html","web")</f>
         <v>0</v>
       </c>
       <c r="H21" s="0" t="s">
@@ -1501,10 +1492,10 @@
         <v>80</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1512,35 +1503,35 @@
         <v>75</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="G22" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6e30ba1e2c19dcbd85faa176d4eae596.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
         <v>0</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1548,7 +1539,7 @@
         <v>75</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>13</v>
@@ -1557,26 +1548,26 @@
         <v>70</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G23" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
         <v>0</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1584,7 +1575,7 @@
         <v>75</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>13</v>
@@ -1593,26 +1584,26 @@
         <v>70</v>
       </c>
       <c r="E24" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="K24" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="K24" s="0" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1620,7 +1611,7 @@
         <v>75</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>13</v>
@@ -1629,26 +1620,26 @@
         <v>70</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="G25" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
         <v>0</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1656,35 +1647,35 @@
         <v>75</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
         <v>0</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,35 +1683,35 @@
         <v>75</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G27" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
         <v>0</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1728,187 +1719,187 @@
         <v>75</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G28" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
         <v>0</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E29" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="F29" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="0" t="s">
+      <c r="B30" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="I29" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="J29" s="0" t="s">
+      <c r="C30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="K29" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="E30" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="F30" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="0" t="s">
+      <c r="G30" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9b495e2-5989-11e6-a4be-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="I30" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="K30" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="G31" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9b495e2-5989-11e6-a4be-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="0" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="I31" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J31" s="0" t="s">
+      <c r="B32" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="K31" s="0" t="s">
+      <c r="C32" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="0" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="E32" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="F32" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="0" t="s">
+      <c r="I32" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="J32" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="F33" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G33" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="0" t="s">
+      <c r="K32" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="I33" s="0" t="s">
+      <c r="B34" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="J33" s="0" t="s">
+      <c r="C34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="K33" s="0" t="s">
-        <v>140</v>
+      <c r="F34" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cfe4bddb7dbbfc57c19837e7f99d2dda.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="K34" s="0" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G35" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cfe4bddb7dbbfc57c19837e7f99d2dda.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a640b0-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
         <v>0</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="I35" s="0" t="s">
         <v>65</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>13</v>
@@ -1917,34 +1908,34 @@
         <v>70</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G36" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a640b0-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a673b4-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
         <v>0</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I36" s="0" t="s">
         <v>65</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>13</v>
@@ -1953,70 +1944,70 @@
         <v>70</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G37" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a673b4-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a56fd2-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
         <v>0</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I37" s="0" t="s">
         <v>65</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E38" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="G38" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a56fd2-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="I38" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="J38" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="K38" s="0" t="s">
+      <c r="E39" s="0" t="s">
         <v>169</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>13</v>
@@ -2025,34 +2016,34 @@
         <v>70</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G40" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="I40" s="0" t="s">
         <v>57</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="K40" s="0" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>13</v>
@@ -2061,34 +2052,34 @@
         <v>70</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="G41" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="I41" s="0" t="s">
         <v>57</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="K41" s="0" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>13</v>
@@ -2097,34 +2088,34 @@
         <v>70</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G42" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="I42" s="0" t="s">
         <v>57</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="K42" s="0" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>13</v>
@@ -2133,34 +2124,34 @@
         <v>70</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="G43" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="I43" s="0" t="s">
         <v>57</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>13</v>
@@ -2169,106 +2160,106 @@
         <v>70</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G44" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I44" s="0" t="s">
         <v>57</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="K45" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E45" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="G45" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="I45" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="J45" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="K45" s="0" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H46" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="I46" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="J46" s="0" t="s">
+      <c r="E47" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="I47" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="K47" s="0" t="s">
         <v>204</v>
-      </c>
-      <c r="K46" s="0" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>13</v>
@@ -2277,34 +2268,34 @@
         <v>70</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G48" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
         <v>0</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>13</v>
@@ -2313,34 +2304,34 @@
         <v>70</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="G49" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
         <v>0</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="K49" s="0" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>13</v>
@@ -2349,386 +2340,350 @@
         <v>70</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="G50" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
         <v>0</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K50" s="0" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G51" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
         <v>0</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="K51" s="0" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F52" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G52" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
         <v>0</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="K52" s="0" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G53" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
         <v>0</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K53" s="0" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="B54" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F54" s="0" t="s">
+      <c r="E55" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="F55" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G54" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H54" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="I54" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="J54" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="K54" s="0" t="s">
+      <c r="G55" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="K55" s="0" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="B56" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>209</v>
-      </c>
       <c r="E56" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F56" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G56" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
         <v>0</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="K56" s="0" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F57" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G57" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
         <v>0</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="K57" s="0" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F58" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G58" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
         <v>0</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K58" s="0" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>128</v>
+        <v>211</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D59" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="F59" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="E59" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="F59" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="G59" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>131</v>
+        <v>214</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>132</v>
+        <v>215</v>
       </c>
       <c r="K59" s="0" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D60" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="F60" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="G60" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H60" s="0" t="s">
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="I60" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="J60" s="0" t="s">
+      <c r="B61" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C61" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="K60" s="0" t="s">
+      <c r="D61" s="0" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G62" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H62" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I62" s="0" t="s">
+      <c r="E61" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H61" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="I61" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="J62" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="K62" s="0" t="s">
-        <v>176</v>
+      <c r="J61" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="K61" s="0" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2736,296 +2691,262 @@
         <v>220</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>86</v>
+        <v>221</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>221</v>
+        <v>13</v>
       </c>
       <c r="D63" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E63" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="E63" s="0" t="s">
-        <v>87</v>
-      </c>
       <c r="F63" s="0" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="G63" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>89</v>
+        <v>223</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>87</v>
+        <v>224</v>
       </c>
       <c r="K63" s="0" t="s">
-        <v>176</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H64" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="K64" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>224</v>
+        <v>12</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>70</v>
+        <v>230</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>225</v>
+        <v>15</v>
       </c>
       <c r="F65" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G65" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>226</v>
+        <v>17</v>
       </c>
       <c r="I65" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>227</v>
+        <v>19</v>
       </c>
       <c r="K65" s="0" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="F66" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G66" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H66" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="I66" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J66" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="K66" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F67" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G67" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H67" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I67" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J67" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K67" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B72" s="2" t="s">
+    <row r="70" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72" s="2" t="s">
+      <c r="C70" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E72" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="F72" s="2" t="s">
+      <c r="E70" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G72" s="2" t="str">
+      <c r="G70" s="2" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917e2ba-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H72" s="2" t="s">
+      <c r="H70" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="I70" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J72" s="2" t="s">
+      <c r="J70" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="K72" s="2" t="s">
+      <c r="K70" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="G73" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/865d0e00-53e6-11e6-b524-5404a60d96b5.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="J73" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="K73" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G74" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J74" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="K74" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>237</v>
+        <v>12</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>143</v>
+        <v>241</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>137</v>
+        <v>16</v>
       </c>
       <c r="G75" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/865d0e00-53e6-11e6-b524-5404a60d96b5.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="J75" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="K75" s="0" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="B76" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="E76" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="F76" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G76" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="J76" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="K76" s="0" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="E77" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="F77" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G77" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H77" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="J77" s="0" t="s">
+      <c r="H75" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J75" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="K77" s="0" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="K75" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Move E3hr prrc from identified missing to ignored list #444.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="237">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -226,228 +226,213 @@
     <t xml:space="preserve">DynVar,VolMIP</t>
   </si>
   <si>
-    <t xml:space="preserve">E3hr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prrc</t>
+    <t xml:space="preserve">CFmon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tntr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude alevel time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tendency of Air Temperature Due to Radiative Heating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.95                                                                Available in IFS: T-tendency from radiation: grib 128.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twan, Thomas &amp; Gijs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tendency of Air Temperature due to Radiative Heating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,CFMIP,DAMIP,GeoMIP,HighResMIP,PMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tnhus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tendency of Specific Humidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grib 126.94 + 126.99 + 126.106 + 126.110  Adding all the q-tendencies, thus: grib 128.94 + 128.99 + 128.106 + 128.110.  Alternatively, in IFS: just estimating the delta q per month. So far no direct grib code for the totoal q-tendency found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tnhusc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tendency of Specific Humidity Due to Convection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.106                                                              Available in IFS: q-tendency from convection: grib 128.106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tnhusmp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tendency of Specific Humidity Due to Model Physics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.99 + 126.106 + 126.110                      Adding all the q-tendencies without advection, thus: grib 128.99 + 128.106 + 128.110.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tendency of specific humidity due to model physics. This includes sources and sinks from parametrized moist physics (e.g. convection, boundary layer, stratiform condensation/evaporation, etc.) and excludes sources and sinks from resolved dynamics or from horizontal or vertical numerical diffusion not associated with model physics.  For example any diffusive mixing by the boundary layer scheme would be included.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cltisccp</t>
   </si>
   <si>
     <t xml:space="preserve">longitude latitude time</t>
   </si>
   <si>
-    <t xml:space="preserve">Convective Rainfall Rate</t>
+    <t xml:space="preserve">ISCCP Total Cloud Cover Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP grib 126.44   CVEXTR2(5)='ISCCP_TOTALCLD'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klaus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage total cloud cover, simulating ISCCP observations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,CFMIP,DAMIP,HighResMIP,PMIP,RFMIP,VIACSAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">albisccp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISCCP Mean Cloud Albedo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP grib 126.46   CVEXTR2(7)='ISCCP_MEANALBCLD'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISCCP Mean Cloud Albedo. Time-means are weighted by the ISCCP Total Cloud Fraction {:cltisccp} - see  http://cfmip.metoffice.com/COSP.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,CFMIP,DAMIP,HighResMIP,RFMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pctisccp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISCCP Mean Cloud Top Pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP grib 126.45   CVEXTR2(6)='ISCCP_MEANPTOP'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISCCP Mean Cloud Top Pressure. Time-means are weighted by the ISCCP Total Cloud Fraction {:cltisccp} - see  http://cfmip.metoffice.com/COSP.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cltcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIPSO Total Cloud Cover Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP grib 126.43   CVEXTR2(4)='CALIPSO_TCC'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'X_area_fraction' means the fraction of horizontal area occupied by X. 'X_area' means the horizontal area occupied by X within the grid cell. Cloud area fraction is also called 'cloud amount' and 'cloud cover'. The cloud area fraction is for the whole atmosphere column, as seen from the surface or the top of the atmosphere. The cloud area fraction in a layer of the atmosphere has the standard name cloud_area_fraction_in_atmosphere_layer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,CFMIP,DAMIP,HighResMIP,RFMIP,VIACSAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cllcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time p840</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIPSO Low Level Cloud Cover Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP grib 126.40   CVEXTR2(1)='CALIPSO_LCC'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage cloud cover in layer centred on 840hPa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clmcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time p560</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIPSO Mid Level Cloud Cover Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP grib 126.41   CVEXTR2(2)='CALIPSO_MCC'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage cloud cover in layer centred on 560hPa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clhcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time p220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIPSO High Level Cloud Area Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP grib 126.42   CVEXTR2(3)='CALIPSO_HCC'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage cloud cover in layer centred on 220hPa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IfxGre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">areacellg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grid-Cell Area for Ice Sheet Variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in PISM. This is the ice sheet mask (in fraction) defined in the ice sheet model grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area of the target grid (not the interpolated area of the source grid).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISMIP6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImonGre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrroLi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xgre ygre time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land Ice Runoff Flux</t>
   </si>
   <si>
     <t xml:space="preserve">kg m-2 s-1</t>
   </si>
   <si>
-    <t xml:space="preserve">Availlable in IFS: Precip. flux from convection liquid grib 128.107, this is a 3D field so the surface field has to be extracted from this. So only level 91 needs to be outputted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In accordance with common usage in geophysical disciplines, 'flux' implies per unit area, called 'flux density' in physics.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CFmon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tntr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude alevel time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tendency of Air Temperature Due to Radiative Heating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grib 126.95                                                                Available in IFS: T-tendency from radiation: grib 128.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Twan, Thomas &amp; Gijs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tendency of Air Temperature due to Radiative Heating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AerChemMIP,CFMIP,DAMIP,GeoMIP,HighResMIP,PMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tnhus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tendency of Specific Humidity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grib 126.94 + 126.99 + 126.106 + 126.110  Adding all the q-tendencies, thus: grib 128.94 + 128.99 + 128.106 + 128.110.  Alternatively, in IFS: just estimating the delta q per month. So far no direct grib code for the totoal q-tendency found</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tnhusc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tendency of Specific Humidity Due to Convection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grib 126.106                                                              Available in IFS: q-tendency from convection: grib 128.106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tnhusmp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tendency of Specific Humidity Due to Model Physics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grib 126.99 + 126.106 + 126.110                      Adding all the q-tendencies without advection, thus: grib 128.99 + 128.106 + 128.110.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tendency of specific humidity due to model physics. This includes sources and sinks from parametrized moist physics (e.g. convection, boundary layer, stratiform condensation/evaporation, etc.) and excludes sources and sinks from resolved dynamics or from horizontal or vertical numerical diffusion not associated with model physics.  For example any diffusive mixing by the boundary layer scheme would be included.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cltisccp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISCCP Total Cloud Cover Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP grib 126.44   CVEXTR2(5)='ISCCP_TOTALCLD'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Klaus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage total cloud cover, simulating ISCCP observations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AerChemMIP,CFMIP,DAMIP,HighResMIP,PMIP,RFMIP,VIACSAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">albisccp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISCCP Mean Cloud Albedo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP grib 126.46   CVEXTR2(7)='ISCCP_MEANALBCLD'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISCCP Mean Cloud Albedo. Time-means are weighted by the ISCCP Total Cloud Fraction {:cltisccp} - see  http://cfmip.metoffice.com/COSP.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AerChemMIP,CFMIP,DAMIP,HighResMIP,RFMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pctisccp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISCCP Mean Cloud Top Pressure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP grib 126.45   CVEXTR2(6)='ISCCP_MEANPTOP'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISCCP Mean Cloud Top Pressure. Time-means are weighted by the ISCCP Total Cloud Fraction {:cltisccp} - see  http://cfmip.metoffice.com/COSP.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cltcalipso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CALIPSO Total Cloud Cover Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP grib 126.43   CVEXTR2(4)='CALIPSO_TCC'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'X_area_fraction' means the fraction of horizontal area occupied by X. 'X_area' means the horizontal area occupied by X within the grid cell. Cloud area fraction is also called 'cloud amount' and 'cloud cover'. The cloud area fraction is for the whole atmosphere column, as seen from the surface or the top of the atmosphere. The cloud area fraction in a layer of the atmosphere has the standard name cloud_area_fraction_in_atmosphere_layer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AerChemMIP,CFMIP,DAMIP,HighResMIP,RFMIP,VIACSAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cllcalipso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time p840</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CALIPSO Low Level Cloud Cover Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP grib 126.40   CVEXTR2(1)='CALIPSO_LCC'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage cloud cover in layer centred on 840hPa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clmcalipso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time p560</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CALIPSO Mid Level Cloud Cover Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP grib 126.41   CVEXTR2(2)='CALIPSO_MCC'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage cloud cover in layer centred on 560hPa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clhcalipso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time p220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CALIPSO High Level Cloud Area Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP grib 126.42   CVEXTR2(3)='CALIPSO_HCC'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage cloud cover in layer centred on 220hPa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IfxGre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">areacellg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grid-Cell Area for Ice Sheet Variables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available in PISM. This is the ice sheet mask (in fraction) defined in the ice sheet model grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area of the target grid (not the interpolated area of the source grid).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISMIP6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ImonGre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrroLi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xgre ygre time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Land Ice Runoff Flux</t>
-  </si>
-  <si>
     <t xml:space="preserve">IFS Surface runoff grib 128.8 but for EC_Earth-GrIs additional melt etc is included</t>
   </si>
   <si>
@@ -713,12 +698,6 @@
   </si>
   <si>
     <t xml:space="preserve">longitude latitude time typegis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Convective Rainfall rate</t>
   </si>
   <si>
     <t xml:space="preserve">IyrGre</t>
@@ -867,8 +846,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A67" activeCellId="0" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1299,28 +1278,64 @@
         <v>71</v>
       </c>
       <c r="F15" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/93a0ba1f23bfc41b720ea68951d28144.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917e2ba-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="0" t="s">
+      <c r="I15" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>65</v>
       </c>
       <c r="J15" s="0" t="s">
         <v>74</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>27</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/52f043533a691ca5721460e316c3a328.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>76</v>
@@ -1329,70 +1344,70 @@
         <v>13</v>
       </c>
       <c r="D17" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="F17" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="0" t="s">
-        <v>63</v>
-      </c>
       <c r="G17" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/93a0ba1f23bfc41b720ea68951d28144.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
         <v>0</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>79</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="G18" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/52f043533a691ca5721460e316c3a328.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d576b3fc447c37d782926441428ffd.html","web")</f>
         <v>0</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J18" s="0" t="s">
         <v>66</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>83</v>
@@ -1401,34 +1416,34 @@
         <v>13</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>84</v>
       </c>
       <c r="F19" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6e30ba1e2c19dcbd85faa176d4eae596.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="G19" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="0" t="s">
+      <c r="I19" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J19" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="I19" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>84</v>
-      </c>
       <c r="K19" s="0" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>87</v>
@@ -1437,286 +1452,250 @@
         <v>13</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="G20" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d576b3fc447c37d782926441428ffd.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
         <v>0</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E21" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="I21" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="F21" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6e30ba1e2c19dcbd85faa176d4eae596.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>80</v>
-      </c>
       <c r="J21" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="G22" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
         <v>0</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J22" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="K22" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G23" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
         <v>0</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="G24" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
         <v>0</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G25" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
         <v>0</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
         <v>0</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>125</v>
@@ -1731,1220 +1710,1151 @@
         <v>127</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="G28" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9b495e2-5989-11e6-a4be-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="K30" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="G30" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9b495e2-5989-11e6-a4be-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J30" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="K30" s="0" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cfe4bddb7dbbfc57c19837e7f99d2dda.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="K32" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="E32" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G32" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="J32" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="K32" s="0" t="s">
-        <v>137</v>
+      <c r="B33" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a640b0-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="K33" s="0" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G34" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cfe4bddb7dbbfc57c19837e7f99d2dda.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a673b4-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
         <v>0</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="I34" s="0" t="s">
         <v>65</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G35" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a640b0-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a56fd2-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
         <v>0</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="I35" s="0" t="s">
         <v>65</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="G36" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a673b4-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="J36" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="K36" s="0" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="B37" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="C37" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="G37" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a56fd2-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="J37" s="0" t="s">
+      <c r="B38" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="F38" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="K37" s="0" t="s">
-        <v>166</v>
+      <c r="G38" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="G39" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="I39" s="0" t="s">
         <v>57</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="E40" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="F40" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="F40" s="0" t="s">
-        <v>170</v>
-      </c>
       <c r="G40" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="I40" s="0" t="s">
         <v>57</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="K40" s="0" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="G41" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="I41" s="0" t="s">
         <v>57</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="K41" s="0" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="E42" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="F42" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="F42" s="0" t="s">
-        <v>180</v>
-      </c>
       <c r="G42" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="I42" s="0" t="s">
         <v>57</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="K42" s="0" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>190</v>
+        <v>13</v>
       </c>
       <c r="G43" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="G44" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H44" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="I44" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="J44" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="K44" s="0" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>167</v>
+        <v>198</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>197</v>
+        <v>87</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="K45" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="B46" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="K46" s="0" t="s">
         <v>199</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="I45" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="J45" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="K45" s="0" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="G47" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
         <v>0</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="K47" s="0" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G48" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
         <v>0</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="G49" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
         <v>0</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="K49" s="0" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G50" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
         <v>0</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="K50" s="0" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G51" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
         <v>0</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="K51" s="0" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H52" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="I52" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="J52" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="K52" s="0" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>126</v>
+        <v>201</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G53" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
         <v>0</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="K53" s="0" t="s">
-        <v>204</v>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="I54" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="K54" s="0" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G55" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
         <v>0</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="K55" s="0" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="B56" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>208</v>
-      </c>
       <c r="E56" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F56" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G56" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
         <v>0</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="K56" s="0" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>120</v>
+        <v>206</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D57" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H57" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="E57" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="F57" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G57" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H57" s="0" t="s">
-        <v>123</v>
-      </c>
       <c r="I57" s="0" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>124</v>
+        <v>210</v>
       </c>
       <c r="K57" s="0" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="F58" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G58" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H58" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="I58" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="J58" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K58" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>211</v>
+        <v>76</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>13</v>
+        <v>213</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>212</v>
+        <v>77</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>213</v>
+        <v>78</v>
       </c>
       <c r="G59" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
         <v>0</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>214</v>
+        <v>79</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>215</v>
+        <v>77</v>
       </c>
       <c r="K59" s="0" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E61" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="B61" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C61" s="0" t="s">
+      <c r="F61" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H61" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="D61" s="0" t="s">
+      <c r="I61" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J61" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="E61" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="F61" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="G61" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H61" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="I61" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J61" s="0" t="s">
-        <v>84</v>
-      </c>
       <c r="K61" s="0" t="s">
-        <v>173</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H62" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="I62" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J62" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="K62" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>221</v>
+        <v>12</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>70</v>
+        <v>225</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>222</v>
+        <v>15</v>
       </c>
       <c r="F63" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G63" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>223</v>
+        <v>17</v>
       </c>
       <c r="I63" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>224</v>
+        <v>19</v>
       </c>
       <c r="K63" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="B64" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="F64" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G64" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H64" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="I64" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J64" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="K64" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F65" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G65" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H65" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I65" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J65" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K65" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G70" s="2" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917e2ba-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J70" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="B73" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E73" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="F73" s="0" t="s">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="G73" s="0" t="str">
+      <c r="E68" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G68" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/865d0e00-53e6-11e6-b524-5404a60d96b5.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H73" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="J73" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="K73" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="H68" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="J68" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="K68" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="E69" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="B74" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="E74" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="F74" s="0" t="s">
+      <c r="F69" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G74" s="0" t="str">
+      <c r="G69" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H74" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="J74" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="K74" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="B75" s="0" t="s">
+      <c r="H69" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="K69" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B70" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C75" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="E75" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="F75" s="0" t="s">
+      <c r="C70" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="F70" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G75" s="0" t="str">
+      <c r="G70" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H75" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="J75" s="0" t="s">
+      <c r="H70" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J70" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="K75" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="K70" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
The comment of the PEXTRA table 126 variables in the (pre) identified missing file has been completed #450.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="254">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">Grounded Ice Sheet Area Percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">For Greenland this is the same as above sftgif. We do not have Antarctic ice sheet.</t>
+    <t xml:space="preserve">To be implemented:  grib 126.30  part of MFPPHY   For Greenland this is the same as above sftgif. We do not have Antarctic ice sheet.</t>
   </si>
   <si>
     <t xml:space="preserve">Shuting</t>
@@ -214,7 +214,7 @@
     <t xml:space="preserve">K s-1</t>
   </si>
   <si>
-    <t xml:space="preserve">grib 126.105                                                              Available in IFS: T-tendency from convection : grib 128.105</t>
+    <t xml:space="preserve">grib 126.105                                                                   part of MFP3D        Available in IFS: T-tendency from convection : grib 128.105</t>
   </si>
   <si>
     <t xml:space="preserve">Twan, Thomas &amp; Gijs</t>
@@ -238,7 +238,7 @@
     <t xml:space="preserve">ISCCP Mean Cloud Albedo</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP grib 126.46   CVEXTR2(7)='ISCCP_MEANALBCLD'</t>
+    <t xml:space="preserve">COSP grib 126.46   CVEXTR2(7)='ISCCP_MEANALBCLD'       part of MFPPHY</t>
   </si>
   <si>
     <t xml:space="preserve">Klaus</t>
@@ -259,7 +259,7 @@
     <t xml:space="preserve">CALIPSO High Level Cloud Area Percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP grib 126.42   CVEXTR2(3)='CALIPSO_HCC'</t>
+    <t xml:space="preserve">COSP grib 126.42   CVEXTR2(3)='CALIPSO_HCC'                part of MFPPHY</t>
   </si>
   <si>
     <t xml:space="preserve">Percentage cloud cover in layer centred on 220hPa</t>
@@ -274,7 +274,7 @@
     <t xml:space="preserve">CALIPSO Low Level Cloud Cover Percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP grib 126.40   CVEXTR2(1)='CALIPSO_LCC'</t>
+    <t xml:space="preserve">COSP grib 126.40   CVEXTR2(1)='CALIPSO_LCC'                part of MFPPHY</t>
   </si>
   <si>
     <t xml:space="preserve">Percentage cloud cover in layer centred on 840hPa</t>
@@ -289,7 +289,7 @@
     <t xml:space="preserve">CALIPSO Mid Level Cloud Cover Percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP grib 126.41   CVEXTR2(2)='CALIPSO_MCC'</t>
+    <t xml:space="preserve">COSP grib 126.41   CVEXTR2(2)='CALIPSO_MCC'               part of MFPPHY</t>
   </si>
   <si>
     <t xml:space="preserve">Percentage cloud cover in layer centred on 560hPa</t>
@@ -301,7 +301,7 @@
     <t xml:space="preserve">CALIPSO Total Cloud Cover Percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP grib 126.43   CVEXTR2(4)='CALIPSO_TCC'</t>
+    <t xml:space="preserve">COSP grib 126.43   CVEXTR2(4)='CALIPSO_TCC'                part of MFPPHY</t>
   </si>
   <si>
     <t xml:space="preserve">'X_area_fraction' means the fraction of horizontal area occupied by X. 'X_area' means the horizontal area occupied by X within the grid cell. Cloud area fraction is also called 'cloud amount' and 'cloud cover'. The cloud area fraction is for the whole atmosphere column, as seen from the surface or the top of the atmosphere. The cloud area fraction in a layer of the atmosphere has the standard name cloud_area_fraction_in_atmosphere_layer.</t>
@@ -316,7 +316,7 @@
     <t xml:space="preserve">ISCCP Total Cloud Cover Percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP grib 126.44   CVEXTR2(5)='ISCCP_TOTALCLD'</t>
+    <t xml:space="preserve">COSP grib 126.44   CVEXTR2(5)='ISCCP_TOTALCLD'       part of MFPPHY</t>
   </si>
   <si>
     <t xml:space="preserve">Percentage total cloud cover, simulating ISCCP observations.</t>
@@ -334,7 +334,7 @@
     <t xml:space="preserve">Pa</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP grib 126.45   CVEXTR2(6)='ISCCP_MEANPTOP'</t>
+    <t xml:space="preserve">COSP grib 126.45   CVEXTR2(6)='ISCCP_MEANPTOP'           part of MFPPHY</t>
   </si>
   <si>
     <t xml:space="preserve">ISCCP Mean Cloud Top Pressure. Time-means are weighted by the ISCCP Total Cloud Fraction {:cltisccp} - see  http://cfmip.metoffice.com/COSP.html</t>
@@ -352,7 +352,7 @@
     <t xml:space="preserve">s-1</t>
   </si>
   <si>
-    <t xml:space="preserve">Grib 126.94 + 126.99 + 126.106 + 126.110  Adding all the q-tendencies, thus: grib 128.94 + 128.99 + 128.106 + 128.110.  Alternatively, in IFS: just estimating the delta q per month. So far no direct grib code for the totoal q-tendency found</t>
+    <t xml:space="preserve">Grib 126.94 + 126.99 + 126.106 + 126.110       part of MFP3D        Adding all the q-tendencies, thus: grib 128.94 + 128.99 + 128.106 + 128.110.  Alternatively, in IFS: just estimating the delta q per month. So far no direct grib code for the totoal q-tendency found</t>
   </si>
   <si>
     <t xml:space="preserve">AerChemMIP,CFMIP,DAMIP,GeoMIP,HighResMIP,PMIP</t>
@@ -364,7 +364,7 @@
     <t xml:space="preserve">Tendency of Specific Humidity Due to Convection</t>
   </si>
   <si>
-    <t xml:space="preserve">grib 126.106                                                              Available in IFS: q-tendency from convection: grib 128.106</t>
+    <t xml:space="preserve">grib 126.106                                                                   part of MFP3D        Available in IFS: q-tendency from convection: grib 128.106</t>
   </si>
   <si>
     <t xml:space="preserve">tnhusmp</t>
@@ -373,7 +373,7 @@
     <t xml:space="preserve">Tendency of Specific Humidity Due to Model Physics</t>
   </si>
   <si>
-    <t xml:space="preserve">grib 126.99 + 126.106 + 126.110                      Adding all the q-tendencies without advection, thus: grib 128.99 + 128.106 + 128.110.</t>
+    <t xml:space="preserve">grib 126.99 + 126.106 + 126.110                           part of MFP3D        Adding all the q-tendencies without advection, thus: grib 128.99 + 128.106 + 128.110.</t>
   </si>
   <si>
     <t xml:space="preserve">Tendency of specific humidity due to model physics. This includes sources and sinks from parametrized moist physics (e.g. convection, boundary layer, stratiform condensation/evaporation, etc.) and excludes sources and sinks from resolved dynamics or from horizontal or vertical numerical diffusion not associated with model physics.  For example any diffusive mixing by the boundary layer scheme would be included.</t>
@@ -385,7 +385,7 @@
     <t xml:space="preserve">Tendency of Air Temperature Due to Radiative Heating</t>
   </si>
   <si>
-    <t xml:space="preserve">grib 126.95                                                                Available in IFS: T-tendency from radiation: grib 128.95</t>
+    <t xml:space="preserve">grib 126.95                                                                      part of MFP3D        Available in IFS: T-tendency from radiation: grib 128.95</t>
   </si>
   <si>
     <t xml:space="preserve">Tendency of Air Temperature due to Radiative Heating</t>
@@ -406,7 +406,7 @@
     <t xml:space="preserve">m2</t>
   </si>
   <si>
-    <t xml:space="preserve">Available in PISM. This is the ice sheet mask (in fraction) defined in the ice sheet model grid</t>
+    <t xml:space="preserve">To be implemented:  grib 126.34  part of MFPPHY   Available in PISM. This is the ice sheet mask (in fraction) defined in the ice sheet model grid</t>
   </si>
   <si>
     <t xml:space="preserve">Area of the target grid (not the interpolated area of the source grid).</t>
@@ -454,7 +454,7 @@
     <t xml:space="preserve">m-3</t>
   </si>
   <si>
-    <t xml:space="preserve">Grib 126.20 / 126.22  in namelist.ifs.cloudact+diag.sh  CVEXTRA(1)='CDNC' which is a PEXTRA variable.</t>
+    <t xml:space="preserve">Grib 126.20 / 126.22        part of MFP3D        In namelist.ifs.cloudact+diag.sh  CVEXTRA(1)='CDNC' which is a PEXTRA variable.</t>
   </si>
   <si>
     <t xml:space="preserve">Twan &amp; Thomas</t>
@@ -475,7 +475,7 @@
     <t xml:space="preserve">W m-2</t>
   </si>
   <si>
-    <t xml:space="preserve">grib 126.73                      Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
+    <t xml:space="preserve">grib 126.73                          part of MFPPHY    Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
   </si>
   <si>
     <t xml:space="preserve">Flux corresponding to rlut resulting from aerosol-free call to radiation, following Ghan (ACP, 2013)</t>
@@ -490,7 +490,7 @@
     <t xml:space="preserve">TOA Outgoing Clear-Sky, Aerosol-Free Longwave Radiation</t>
   </si>
   <si>
-    <t xml:space="preserve">grib 126.72                       Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
+    <t xml:space="preserve">grib 126.72                          part of MFPPHY    Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
   </si>
   <si>
     <t xml:space="preserve">Flux corresponding to rlutcs resulting from aerosol-free call to radiation, following Ghan (ACP, 2013)</t>
@@ -502,7 +502,7 @@
     <t xml:space="preserve">TOA Outgoing Aerosol-Free Shortwave Radiation</t>
   </si>
   <si>
-    <t xml:space="preserve">grib 128.212-126.069  Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
+    <t xml:space="preserve">grib 128.212-126.069     part of MFPPHY    Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
   </si>
   <si>
     <t xml:space="preserve">Flux corresponding to rsut resulting from aerosol-free call to radiation, following Ghan (ACP, 2013)</t>
@@ -688,88 +688,91 @@
     <t xml:space="preserve">Land Ice Area Percentage</t>
   </si>
   <si>
+    <t xml:space="preserve">To be implemented:  grib 126.32  part of MFPPHY   This is the land ice mask and will be an extra variable in IFS (thomas: via PEXTRA?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraction of grid cell covered by land ice (ice sheet, ice shelf, ice cap, glacier)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time typegis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sncIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Sheet Snow Cover Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To be implemented:  grib 126.31  part of MFPPHY   Not available in IFS. Although it could be calculated from tile fractions and written out as extra output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of each grid cell that is occupied by snow that rests on land portion of cell.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CFsubhr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">degrees_north</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This site lon,lat is specifed by the experiment we guess, and should be available in the netcdf file. So far it doesn't seem to be specified in the data request: in the CMIP6_coordinate.json table file the requested": "" is empty for site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latitude is positive northward; its units of degree_north (or equivalent) indicate this explicitly. In a latitude-longitude system defined with respect to a rotated North Pole, the standard name of grid_latitude should be used instead of latitude. Grid latitude is positive in the grid-northward direction, but its units should be plain degree.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,CFMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">degrees_east</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitude is positive eastward; its units of degree_east (or equivalent) indicate this explicitly. In a latitude-longitude system defined with respect to a rotated North Pole, the standard name of grid_longitude should be used instead of longitude. Grid longitude is positive in the grid-eastward direction, but its units should be plain degree.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alevel site time1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IyrGre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modelCellAreai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cell area of the ice sheet model.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PISM model probably uses a constant and uniform grid size within EC-Earth, this grid size can be reported or a filed from the grid sizes can be provided in a post processing phase.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal area of ice-sheet grid cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xgre ygre time typeli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraction of Grid Cell Covered with Glacier</t>
+  </si>
+  <si>
     <t xml:space="preserve">This is the land ice mask and will be an extra variable in IFS (thomas: via PEXTRA?)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fraction of grid cell covered by land ice (ice sheet, ice shelf, ice cap, glacier)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time typegis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sncIs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ice Sheet Snow Cover Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not available in IFS. Although it could be calculated from tile fractions and written out as extra output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of each grid cell that is occupied by snow that rests on land portion of cell.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CFsubhr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">degrees_north</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This site lon,lat is specifed by the experiment we guess, and should be available in the netcdf file. So far it doesn't seem to be specified in the data request: in the CMIP6_coordinate.json table file the requested": "" is empty for site.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latitude is positive northward; its units of degree_north (or equivalent) indicate this explicitly. In a latitude-longitude system defined with respect to a rotated North Pole, the standard name of grid_latitude should be used instead of latitude. Grid latitude is positive in the grid-northward direction, but its units should be plain degree.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AerChemMIP,CFMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Longitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">degrees_east</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Longitude is positive eastward; its units of degree_east (or equivalent) indicate this explicitly. In a latitude-longitude system defined with respect to a rotated North Pole, the standard name of grid_longitude should be used instead of longitude. Grid longitude is positive in the grid-eastward direction, but its units should be plain degree.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alevel site time1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IyrGre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modelCellAreai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cell area of the ice sheet model.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The PISM model probably uses a constant and uniform grid size within EC-Earth, this grid size can be reported or a filed from the grid sizes can be provided in a post processing phase.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horizontal area of ice-sheet grid cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xgre ygre time typeli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fraction of Grid Cell Covered with Glacier</t>
   </si>
   <si>
     <t xml:space="preserve">xgre ygre time typegis</t>
@@ -894,7 +897,7 @@
   </sheetPr>
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="76:83"/>
     </sheetView>
   </sheetViews>
@@ -3173,7 +3176,7 @@
         <v>web</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>137</v>
@@ -3196,10 +3199,10 @@
         <v>13</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F82" s="0" t="s">
         <v>22</v>
@@ -3209,7 +3212,7 @@
         <v>web</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>137</v>

</xml_diff>

<commit_message>
The Amon o3 combination will be added to the identified missing list in order to prevent IFS crashes, and to pave the way for release 1.0.0 #458 #440.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="253">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -810,6 +810,33 @@
   </si>
   <si>
     <t xml:space="preserve">A nudging increment refers to an amount added to parts of a model system. The phrase 'nudging_increment_in_X' refers to an increment in quantity X over a time period which should be defined in the bounds of the time coordinate. The surface called 'surface' means the lower boundary of the atmosphere. 'Amount' means mass per unit area. 'Snow and ice on land' means ice in glaciers, ice caps, ice sheets &amp; shelves, river and lake ice, any other ice on a land surface, such as frozen flood water, and snow lying on such ice or on the land surface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude plev19 time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mole Fraction of O3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mol mol-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tm5 code name = o3|ifs code name = 203.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automatic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mole fraction is used in the construction mole_fraction_of_X_in_Y, where X is a material constituent of Y.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,C4MIP,CFMIP,CMIP,DAMIP,FAFMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,LUMIP,RFMIP,VolMIP</t>
   </si>
 </sst>
 </file>
@@ -992,8 +1019,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A78" activeCellId="0" sqref="78:78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3067,6 +3094,42 @@
       </c>
       <c r="K75" s="0" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="78" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G78" s="2" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1d4594c97188efd47935238a429e02e4.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="K78" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Using drq2ppt with the --allvars caused problematic ppt files because 126-table variables ended up in the ppt for the mode without the 126 table. A few variable-table combinations had to be traced and have been added manually to the list-of-identified-missing so they will not longer mesh up the produced ppt files #474.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="248">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -780,6 +780,48 @@
   </si>
   <si>
     <t xml:space="preserve">AerChemMIP,C4MIP,CFMIP,CMIP,DAMIP,FAFMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,LUMIP,RFMIP,VolMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vtendogw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northward Acceleration Due to Orographic Gravity Wave Drag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m s-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tendency of the northward wind by parameterized orographic gravity waves.  (Note that CF name tables only have a general northward tendency for all gravity waves, and we need it separated by type.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vtendnogw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northward Acceleration Due to Non-Orographic Gravity Wave Drag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tendency of the northward wind by parameterized nonorographic gravity waves.  (Note that CF name tables only have a general northward tendency for all gravity waves, and we need it separated by type.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tntogw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature Tendency Due to Orographic Gravity Wave Dissipation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature tendency due to dissipation of parameterized orographic gravity waves.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tntnogw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature Tendency Due to Non-Orographic Gravity Wave Dissipation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature tendency due to dissipation of parameterized nonorographic gravity waves.</t>
   </si>
 </sst>
 </file>
@@ -962,8 +1004,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C80" activeCellId="0" sqref="C80:C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2887,6 +2929,157 @@
         <v>233</v>
       </c>
     </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G78" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H78" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="I78" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J78" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="K78" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="G81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J83" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" s="0" t="s">
+        <v>247</v>
+      </c>
+    </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Removing tsland and mrsow from the pre identified missing and the identified missing lists, so they become available #394.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="239">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -708,36 +708,6 @@
   </si>
   <si>
     <t xml:space="preserve">A nudging increment refers to an amount added to parts of a model system. The phrase 'nudging_increment_in_X' refers to an increment in quantity X over a time period which should be defined in the bounds of the time coordinate. The surface called 'surface' means the lower boundary of the atmosphere. 'Amount' means mass per unit area. 'Snow and ice on land' means ice in glaciers, ice caps, ice sheets &amp; shelves, river and lake ice, any other ice on a land surface, such as frozen flood water, and snow lying on such ice or on the land surface.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrsow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Soil Wetness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrsow=swvl1*0.07+swvl2*0.21+swvl3*0.72+swvl4*1.89 note: NOT divided by maximum allowable soil moisture above wilting point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrea Alessandri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically integrated soil moisture divided by maximum allowable soil moisture above wilting point.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tsland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Land Surface Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available by IFS: grib code 235 but it needs masking out the ocean points: thus add in ifspar.json the entry "masked": "land"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature of the lower boundary of the atmosphere</t>
   </si>
   <si>
     <t xml:space="preserve">Amon</t>
@@ -1001,10 +971,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K83"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1018,7 +988,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
@@ -2747,304 +2717,238 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>32</v>
+        <v>212</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>13</v>
+        <v>214</v>
       </c>
       <c r="G70" s="0" t="s">
         <v>186</v>
       </c>
       <c r="H70" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="I70" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="J70" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="K70" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="H73" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="I73" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J73" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="K73" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="D75" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="I70" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="J70" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="K70" s="0" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="F71" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="G71" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="H71" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="I71" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="J71" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="K71" s="0" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="B74" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D74" s="0" t="s">
+      <c r="E75" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="G75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="J75" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="K75" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C76" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="E74" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="F74" s="0" t="s">
+      <c r="D76" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="F76" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="G74" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="H74" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="I74" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="J74" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="K74" s="0" t="s">
-        <v>228</v>
+      <c r="G76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="J76" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="K76" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>229</v>
+        <v>21</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>175</v>
+        <v>221</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>13</v>
+        <v>222</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>230</v>
+        <v>23</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>176</v>
+        <v>223</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G77" s="0" t="s">
-        <v>186</v>
+        <v>224</v>
+      </c>
+      <c r="G77" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="I77" s="0" t="s">
-        <v>18</v>
+        <v>225</v>
       </c>
       <c r="J77" s="0" t="s">
-        <v>193</v>
+        <v>226</v>
       </c>
       <c r="K77" s="0" t="s">
-        <v>20</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="J78" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="K78" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>123</v>
+        <v>21</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>222</v>
+        <v>23</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>234</v>
+        <v>25</v>
       </c>
       <c r="G79" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="J79" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="K79" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="B80" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="D80" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="E80" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="F80" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="G80" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H80" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="J80" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="K80" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B81" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="D81" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E81" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="F81" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="G81" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H81" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="J81" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="K81" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B82" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E82" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="F82" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="G82" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H82" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="J82" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="K82" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B83" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E83" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="F83" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="G83" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H83" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="J83" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="K83" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Reprocess the identification process - achieving an emty missing list for the step 1+2 case! #554.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="242">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -542,6 +542,15 @@
   </si>
   <si>
     <t xml:space="preserve">RFMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esubhr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude alevel time1</t>
   </si>
   <si>
     <t xml:space="preserve">LImon</t>
@@ -973,11 +982,11 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H75" activeCellId="0" sqref="H75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -988,12 +997,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1037,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
@@ -1064,7 +1073,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>21</v>
       </c>
@@ -1100,7 +1109,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>30</v>
       </c>
@@ -1136,7 +1145,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>30</v>
       </c>
@@ -1172,7 +1181,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>30</v>
       </c>
@@ -1208,7 +1217,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>30</v>
       </c>
@@ -1244,7 +1253,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>30</v>
       </c>
@@ -1280,7 +1289,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>30</v>
       </c>
@@ -1316,7 +1325,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>30</v>
       </c>
@@ -1352,7 +1361,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>30</v>
       </c>
@@ -1388,7 +1397,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>30</v>
       </c>
@@ -1424,7 +1433,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>30</v>
       </c>
@@ -1460,7 +1469,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>30</v>
       </c>
@@ -1496,7 +1505,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>30</v>
       </c>
@@ -1532,7 +1541,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>85</v>
       </c>
@@ -1568,7 +1577,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>92</v>
       </c>
@@ -1604,7 +1613,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>100</v>
       </c>
@@ -1640,7 +1649,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>100</v>
       </c>
@@ -1676,7 +1685,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>100</v>
       </c>
@@ -1712,7 +1721,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>100</v>
       </c>
@@ -1748,7 +1757,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>123</v>
       </c>
@@ -1784,7 +1793,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>123</v>
       </c>
@@ -1820,7 +1829,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>123</v>
       </c>
@@ -1856,7 +1865,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>123</v>
       </c>
@@ -1892,7 +1901,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>123</v>
       </c>
@@ -1928,7 +1937,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>123</v>
       </c>
@@ -1964,7 +1973,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>123</v>
       </c>
@@ -2000,7 +2009,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>160</v>
       </c>
@@ -2036,7 +2045,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>160</v>
       </c>
@@ -2072,7 +2081,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>160</v>
       </c>
@@ -2108,7 +2117,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>160</v>
       </c>
@@ -2144,7 +2153,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>160</v>
       </c>
@@ -2180,7 +2189,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>160</v>
       </c>
@@ -2216,7 +2225,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>160</v>
       </c>
@@ -2252,7 +2261,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>162</v>
       </c>
@@ -2288,7 +2297,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>162</v>
       </c>
@@ -2324,7 +2333,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>162</v>
       </c>
@@ -2360,7 +2369,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>162</v>
       </c>
@@ -2396,7 +2405,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>162</v>
       </c>
@@ -2432,84 +2441,48 @@
         <v>173</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>174</v>
       </c>
       <c r="B51" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="C51" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="D51" s="0" t="s">
-        <v>32</v>
+        <v>176</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>176</v>
+        <v>70</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="G51" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
         <v>0</v>
       </c>
       <c r="H51" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="K51" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="I51" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J51" s="0" t="s">
+      <c r="B53" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="K51" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H52" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I52" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J52" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K52" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>179</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>13</v>
@@ -2518,396 +2491,418 @@
         <v>32</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G53" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
         <v>0</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I53" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J53" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="K53" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I54" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K54" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B55" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="K53" s="0" t="s">
+      <c r="C55" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="K55" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="B61" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="F61" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G61" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="H61" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="I61" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="J61" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="K61" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G62" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="H62" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="I62" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="J62" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="K62" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>12</v>
+        <v>187</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>194</v>
+        <v>94</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>98</v>
+        <v>191</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="K63" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="H64" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="K64" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="E65" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="F65" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="H65" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="C66" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66" s="0" t="s">
+      <c r="I65" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="K65" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E66" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="F66" s="0" t="s">
+      <c r="E68" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="H68" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="I68" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="J68" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="K68" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="G66" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="H66" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="I66" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="J66" s="0" t="s">
+      <c r="B69" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="F69" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="K66" s="0" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="B67" s="0" t="s">
+      <c r="G69" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="H69" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="I69" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="C67" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="F67" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="G67" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="H67" s="0" t="s">
+      <c r="J69" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="K69" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="I67" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="J67" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="K67" s="0" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="B70" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="E70" s="0" t="s">
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="F70" s="0" t="s">
+      <c r="B72" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="G70" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="H70" s="0" t="s">
+      <c r="C72" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="I70" s="0" t="s">
+      <c r="E72" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="J70" s="0" t="s">
+      <c r="F72" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="K70" s="0" t="s">
+      <c r="G72" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="H72" s="0" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="I72" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B73" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73" s="0" t="s">
+      <c r="J72" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="E73" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="F73" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G73" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="H73" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="I73" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J73" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="K73" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
+      <c r="K72" s="0" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>123</v>
+        <v>222</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>222</v>
+        <v>13</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>223</v>
+        <v>179</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="G75" s="0" t="n">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>189</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>225</v>
+        <v>180</v>
+      </c>
+      <c r="I75" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="J75" s="0" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
       <c r="K75" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="B76" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="E76" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="F76" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="G76" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H76" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="J76" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="K76" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>23</v>
+        <v>215</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="G77" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="J77" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="K77" s="0" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="B78" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="E78" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="C78" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E78" s="0" t="s">
+      <c r="F78" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="G78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="F78" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="G78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H78" s="0" t="s">
+      <c r="J78" s="0" t="s">
         <v>233</v>
-      </c>
-      <c r="J78" s="0" t="s">
-        <v>234</v>
       </c>
       <c r="K78" s="0" t="s">
         <v>29</v>
@@ -2918,33 +2913,107 @@
         <v>21</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>23</v>
       </c>
       <c r="E79" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="G79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="J79" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="K79" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="F79" s="0" t="s">
+      <c r="J80" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="K80" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="F81" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="G79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H79" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="J79" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="K79" s="0" t="s">
+      <c r="G81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="J81" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="K81" s="0" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add AERmon rsutcsaf to the identified missing and pre identified missing lists, because its grib code should not end up in the ppt files if PEXTRA is deactivated #556.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="246">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -389,6 +389,18 @@
   </si>
   <si>
     <t xml:space="preserve">AerChemMIP,DAMIP,GeoMIP,HighResMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsutcsaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOA Outgoing Clear-Sky, Aerosol-Free Shortwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 68.126    part of MFPPHY    Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flux corresponding to rsutcs resulting from aerosol-free call to radiation, following Ghan (ACP, 2013)</t>
   </si>
   <si>
     <t xml:space="preserve">Emon</t>
@@ -894,12 +906,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -982,8 +998,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H75" activeCellId="0" sqref="H75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -997,7 +1013,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
@@ -1721,7 +1737,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>100</v>
       </c>
@@ -1757,48 +1773,48 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="28" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="C28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="0" t="s">
+      <c r="F28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G28" s="2" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="I28" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G29" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="J29" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K29" s="0" t="s">
-        <v>130</v>
+      <c r="K28" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>13</v>
@@ -1807,34 +1823,34 @@
         <v>32</v>
       </c>
       <c r="E30" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="I30" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="J30" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="G30" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="0" t="s">
+      <c r="K30" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="J30" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="K30" s="0" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>13</v>
@@ -1843,31 +1859,31 @@
         <v>32</v>
       </c>
       <c r="E31" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="F31" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="F31" s="0" t="s">
-        <v>126</v>
-      </c>
       <c r="G31" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>138</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="J31" s="0" t="s">
         <v>139</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>140</v>
@@ -1882,28 +1898,28 @@
         <v>141</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G32" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H32" s="0" t="s">
         <v>142</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="J32" s="0" t="s">
         <v>143</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>144</v>
@@ -1912,73 +1928,73 @@
         <v>13</v>
       </c>
       <c r="D33" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="F33" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="F33" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="0" t="s">
+      <c r="I33" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J33" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="I33" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="J33" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="K33" s="0" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="C34" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E34" s="0" t="s">
+      <c r="F34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="I34" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="J34" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="G34" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="0" t="s">
+      <c r="K34" s="0" t="s">
         <v>153</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="J34" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="K34" s="0" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>13</v>
@@ -1987,214 +2003,214 @@
         <v>32</v>
       </c>
       <c r="E35" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F35" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="G35" s="0" t="n">
+      <c r="I35" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="G36" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
-      <c r="H35" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="J35" s="0" t="s">
+      <c r="H36" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="K36" s="0" t="s">
         <v>159</v>
-      </c>
-      <c r="K35" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="J37" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="K37" s="0" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G38" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
         <v>0</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I38" s="0" t="s">
         <v>35</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="K38" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G39" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
         <v>0</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I39" s="0" t="s">
         <v>35</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G40" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
         <v>0</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I40" s="0" t="s">
         <v>35</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="K40" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G41" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
         <v>0</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I41" s="0" t="s">
         <v>35</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K41" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>13</v>
@@ -2203,34 +2219,34 @@
         <v>32</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G42" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
         <v>0</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I42" s="0" t="s">
         <v>35</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K42" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>13</v>
@@ -2239,286 +2255,286 @@
         <v>32</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="G43" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
         <v>0</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I43" s="0" t="s">
         <v>35</v>
       </c>
       <c r="J43" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J44" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="K43" s="0" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G45" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I45" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="J45" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="K45" s="0" t="s">
-        <v>164</v>
+      <c r="K44" s="0" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F46" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G46" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
         <v>0</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I46" s="0" t="s">
         <v>35</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K46" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F47" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G47" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
         <v>0</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I47" s="0" t="s">
         <v>35</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="K47" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G48" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
         <v>0</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I48" s="0" t="s">
         <v>35</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B49" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="K49" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="C49" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="G49" s="0" t="n">
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="G50" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
-      <c r="H49" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="I49" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="J49" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="K49" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="B51" s="0" t="s">
+      <c r="H50" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="K50" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B52" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C51" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="E51" s="0" t="s">
+      <c r="C52" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="E52" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="F51" s="0" t="s">
+      <c r="F52" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="G51" s="0" t="n">
+      <c r="G52" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
         <v>0</v>
       </c>
-      <c r="H51" s="0" t="s">
+      <c r="H52" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="I51" s="0" t="s">
+      <c r="I52" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="J51" s="0" t="s">
+      <c r="J52" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="K51" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G53" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H53" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="I53" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J53" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="K53" s="0" t="s">
-        <v>20</v>
+      <c r="K52" s="0" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>12</v>
+        <v>182</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>13</v>
@@ -2527,23 +2543,23 @@
         <v>32</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>15</v>
+        <v>183</v>
       </c>
       <c r="F54" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G54" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
         <v>0</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>17</v>
+        <v>184</v>
       </c>
       <c r="I54" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>19</v>
+        <v>185</v>
       </c>
       <c r="K54" s="0" t="s">
         <v>20</v>
@@ -2551,10 +2567,10 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>182</v>
+        <v>12</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>13</v>
@@ -2563,97 +2579,98 @@
         <v>32</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>183</v>
+        <v>15</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G55" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>184</v>
+        <v>17</v>
       </c>
       <c r="I55" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>185</v>
+        <v>19</v>
       </c>
       <c r="K55" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="K56" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="B63" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="F63" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G63" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="H63" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="I63" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="J63" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="K63" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D64" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G64" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="E64" s="0" t="s">
+      <c r="H64" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="F64" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G64" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="H64" s="0" t="s">
+      <c r="I64" s="0" t="s">
         <v>195</v>
-      </c>
-      <c r="I64" s="0" t="s">
-        <v>98</v>
       </c>
       <c r="J64" s="0" t="s">
         <v>196</v>
@@ -2664,10 +2681,10 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>12</v>
+        <v>182</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>13</v>
@@ -2682,7 +2699,7 @@
         <v>16</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H65" s="0" t="s">
         <v>199</v>
@@ -2697,49 +2714,49 @@
         <v>91</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="H66" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="K66" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="F68" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="G68" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="H68" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="I68" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="J68" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="K68" s="0" t="s">
-        <v>208</v>
-      </c>
-    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>13</v>
@@ -2748,152 +2765,155 @@
         <v>32</v>
       </c>
       <c r="E69" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="H69" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="I69" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="F69" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="G69" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="H69" s="0" t="s">
+      <c r="J69" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="I69" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="J69" s="0" t="s">
+      <c r="K69" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="K69" s="0" t="s">
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="F70" s="0" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="G70" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="H70" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="I70" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="J70" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="K70" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="B72" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="F72" s="0" t="s">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="G72" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="H72" s="0" t="s">
+      <c r="B73" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="I72" s="0" t="s">
+      <c r="C73" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="J72" s="0" t="s">
+      <c r="E73" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="K72" s="0" t="s">
+      <c r="F73" s="0" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="G73" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="H73" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="I73" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="J73" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="K73" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="B75" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="E75" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="F75" s="0" t="s">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F76" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G75" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="H75" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="I75" s="0" t="s">
+      <c r="G76" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="H76" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="I76" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="J75" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="K75" s="0" t="s">
+      <c r="J76" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="K76" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="E77" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="F77" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="G77" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H77" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="J77" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="K77" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B78" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="E78" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="C78" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="E78" s="0" t="s">
+      <c r="F78" s="0" t="s">
         <v>231</v>
-      </c>
-      <c r="F78" s="0" t="s">
-        <v>227</v>
       </c>
       <c r="G78" s="0" t="n">
         <v>0</v>
@@ -2910,34 +2930,34 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>21</v>
+        <v>127</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>23</v>
+        <v>219</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="G79" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="J79" s="0" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="K79" s="0" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2945,31 +2965,31 @@
         <v>21</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D80" s="0" t="s">
         <v>23</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>25</v>
+        <v>231</v>
       </c>
       <c r="G80" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="J80" s="0" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="K80" s="0" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2980,7 +3000,7 @@
         <v>238</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>23</v>
@@ -3004,9 +3024,40 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="J82" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="K82" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add the Emon, CF3hr & Esubhr reffclws combinations of this pextra variable to the missing identified list #564.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="249">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -816,6 +816,15 @@
   </si>
   <si>
     <t xml:space="preserve">Temperature tendency due to dissipation of parameterized orographic gravity waves.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reffclws</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From the AerChem side there is interest in Emon reffclws. This variable is identified as the already available PEXTRA variable with the table 126 grib code 126021, i.e. proposing to add reffclws as 21.126 to ifspar.json.  Note that this variable is not requested by CMIP6 AerChem, and that reffclws not occurs in any CMIP6 data request of the experiments in which any EC-Earth3* configuration participates. See further #564.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CF3hr</t>
   </si>
 </sst>
 </file>
@@ -906,7 +915,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -917,6 +926,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -998,8 +1011,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A85" activeCellId="0" sqref="A85:I87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3058,6 +3071,48 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H85" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="I85" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H86" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="I86" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H87" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="I87" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update the identified missing and ignored lists for cmip6 data request version 01.00.32 #626.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="249">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -538,6 +538,9 @@
     <t xml:space="preserve">longitude latitude time1</t>
   </si>
   <si>
+    <t xml:space="preserve">RFMIP</t>
+  </si>
+  <si>
     <t xml:space="preserve">sza</t>
   </si>
   <si>
@@ -551,9 +554,6 @@
   </si>
   <si>
     <t xml:space="preserve">The angle between the line of sight to the sun and the local vertical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RFMIP</t>
   </si>
   <si>
     <t xml:space="preserve">Esubhr</t>
@@ -915,16 +915,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1011,8 +1007,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A85" activeCellId="0" sqref="A85:I87"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1026,7 +1022,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
@@ -1750,7 +1746,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>100</v>
       </c>
@@ -1786,39 +1782,39 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C28" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="G28" s="2" t="str">
+      <c r="G28" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="0" t="s">
         <v>125</v>
       </c>
       <c r="I28" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="J28" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="K28" s="0" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2475,7 +2471,7 @@
         <v>166</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>172</v>
+        <v>123</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>13</v>
@@ -2484,98 +2480,98 @@
         <v>171</v>
       </c>
       <c r="E50" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="K50" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B51" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="F50" s="0" t="s">
+      <c r="C51" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E51" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="G50" s="0" t="n">
+      <c r="F51" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="G51" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
-      <c r="H50" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="I50" s="0" t="s">
+      <c r="H51" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="I51" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="J50" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="K50" s="0" t="s">
+      <c r="J51" s="0" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="K51" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B53" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C53" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D53" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="E52" s="0" t="s">
+      <c r="E53" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="F52" s="0" t="s">
+      <c r="F53" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="G52" s="0" t="n">
+      <c r="G53" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
         <v>0</v>
       </c>
-      <c r="H52" s="0" t="s">
+      <c r="H53" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="I52" s="0" t="s">
+      <c r="I53" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="J52" s="0" t="s">
+      <c r="J53" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="K52" s="0" t="s">
+      <c r="K53" s="0" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="B54" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="F54" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G54" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H54" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="I54" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J54" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="K54" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2583,7 +2579,7 @@
         <v>181</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>12</v>
+        <v>182</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>13</v>
@@ -2592,23 +2588,23 @@
         <v>32</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>15</v>
+        <v>183</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G55" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
         <v>0</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>17</v>
+        <v>184</v>
       </c>
       <c r="I55" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>19</v>
+        <v>185</v>
       </c>
       <c r="K55" s="0" t="s">
         <v>20</v>
@@ -2619,7 +2615,7 @@
         <v>181</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>13</v>
@@ -2628,100 +2624,101 @@
         <v>32</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>187</v>
+        <v>15</v>
       </c>
       <c r="F56" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G56" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>188</v>
+        <v>17</v>
       </c>
       <c r="I56" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J56" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K56" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="I57" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J57" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="K56" s="0" t="s">
+      <c r="K57" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="B64" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="F64" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G64" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="H64" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="I64" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="J64" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="K64" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>190</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>197</v>
+        <v>94</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="G65" s="0" t="s">
         <v>193</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>98</v>
+        <v>195</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="K65" s="0" t="s">
         <v>91</v>
@@ -2732,16 +2729,16 @@
         <v>190</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>12</v>
+        <v>182</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F66" s="0" t="s">
         <v>16</v>
@@ -2750,61 +2747,61 @@
         <v>193</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I66" s="0" t="s">
         <v>98</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="K66" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="H67" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="I67" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J67" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="K67" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="B69" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="F69" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="G69" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="H69" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="I69" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="J69" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="K69" s="0" t="s">
-        <v>212</v>
-      </c>
-    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>205</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>13</v>
@@ -2813,7 +2810,7 @@
         <v>32</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F70" s="0" t="s">
         <v>208</v>
@@ -2822,131 +2819,134 @@
         <v>193</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="I70" s="0" t="s">
         <v>210</v>
       </c>
       <c r="J70" s="0" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="K70" s="0" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="H71" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="I71" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="J71" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="K71" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B74" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="C73" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73" s="0" t="s">
+      <c r="C74" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="E73" s="0" t="s">
+      <c r="E74" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="F73" s="0" t="s">
+      <c r="F74" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="G73" s="0" t="s">
+      <c r="G74" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="H73" s="0" t="s">
+      <c r="H74" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="I73" s="0" t="s">
+      <c r="I74" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="J73" s="0" t="s">
+      <c r="J74" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="K73" s="0" t="s">
+      <c r="K74" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B77" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="C76" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D76" s="0" t="s">
+      <c r="C77" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E76" s="0" t="s">
+      <c r="E77" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="F76" s="0" t="s">
+      <c r="F77" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G76" s="0" t="s">
+      <c r="G77" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="H76" s="0" t="s">
+      <c r="H77" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="I76" s="0" t="s">
+      <c r="I77" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="J76" s="0" t="s">
+      <c r="J77" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="K76" s="0" t="s">
+      <c r="K77" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B78" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="E78" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="F78" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="G78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H78" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="J78" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="K78" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>127</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C79" s="0" t="s">
         <v>229</v>
@@ -2955,7 +2955,7 @@
         <v>219</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F79" s="0" t="s">
         <v>231</v>
@@ -2964,10 +2964,10 @@
         <v>0</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="J79" s="0" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="K79" s="0" t="s">
         <v>29</v>
@@ -2975,19 +2975,19 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>21</v>
+        <v>127</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C80" s="0" t="s">
         <v>229</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>23</v>
+        <v>219</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="F80" s="0" t="s">
         <v>231</v>
@@ -2996,13 +2996,13 @@
         <v>0</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="J80" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="K80" s="0" t="s">
-        <v>159</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3010,7 +3010,7 @@
         <v>21</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>229</v>
@@ -3019,22 +3019,22 @@
         <v>23</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>25</v>
+        <v>231</v>
       </c>
       <c r="G81" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="J81" s="0" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="K81" s="0" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3042,7 +3042,7 @@
         <v>21</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C82" s="0" t="s">
         <v>229</v>
@@ -3051,7 +3051,7 @@
         <v>23</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F82" s="0" t="s">
         <v>25</v>
@@ -3060,36 +3060,54 @@
         <v>0</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="J82" s="0" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="K82" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="J83" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="K83" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H85" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="I85" s="0" t="s">
-        <v>195</v>
-      </c>
-    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="B86" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>246</v>
       </c>
       <c r="H86" s="0" t="s">
@@ -3101,9 +3119,9 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="B87" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>246</v>
       </c>
       <c r="H87" s="0" t="s">
@@ -3113,6 +3131,22 @@
         <v>195</v>
       </c>
     </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="H88" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="I88" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update the identified missing lists (a forgottn save) for cmip6 data request version 01.00.32 #626.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="246">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -554,15 +554,6 @@
   </si>
   <si>
     <t xml:space="preserve">The angle between the line of sight to the sun and the local vertical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esubhr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude alevel time1</t>
   </si>
   <si>
     <t xml:space="preserve">LImon</t>
@@ -1007,11 +998,11 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -1027,7 +1018,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1053,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
@@ -1081,9 +1072,9 @@
       <c r="F3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>17</v>
@@ -1098,7 +1089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>21</v>
       </c>
@@ -1117,9 +1108,9 @@
       <c r="F5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/52f043533a691ca5721460e316c3a328.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>26</v>
@@ -1134,7 +1125,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>30</v>
       </c>
@@ -1153,9 +1144,9 @@
       <c r="F7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>34</v>
@@ -1170,7 +1161,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>30</v>
       </c>
@@ -1189,9 +1180,9 @@
       <c r="F8" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>41</v>
@@ -1206,7 +1197,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>30</v>
       </c>
@@ -1225,9 +1216,9 @@
       <c r="F9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>46</v>
@@ -1242,7 +1233,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>30</v>
       </c>
@@ -1261,9 +1252,9 @@
       <c r="F10" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>51</v>
@@ -1278,7 +1269,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>30</v>
       </c>
@@ -1297,9 +1288,9 @@
       <c r="F11" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>55</v>
@@ -1314,7 +1305,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>30</v>
       </c>
@@ -1333,9 +1324,9 @@
       <c r="F12" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>60</v>
@@ -1350,7 +1341,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>30</v>
       </c>
@@ -1369,9 +1360,9 @@
       <c r="F13" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>66</v>
@@ -1386,7 +1377,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>30</v>
       </c>
@@ -1405,9 +1396,9 @@
       <c r="F14" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>72</v>
@@ -1422,7 +1413,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>30</v>
       </c>
@@ -1441,9 +1432,9 @@
       <c r="F15" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d576b3fc447c37d782926441428ffd.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>76</v>
@@ -1458,7 +1449,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>30</v>
       </c>
@@ -1477,9 +1468,9 @@
       <c r="F16" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6e30ba1e2c19dcbd85faa176d4eae596.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>79</v>
@@ -1494,7 +1485,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>30</v>
       </c>
@@ -1513,9 +1504,9 @@
       <c r="F17" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/52f043533a691ca5721460e316c3a328.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>26</v>
@@ -1530,7 +1521,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>30</v>
       </c>
@@ -1549,9 +1540,9 @@
       <c r="F18" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/93a0ba1f23bfc41b720ea68951d28144.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>83</v>
@@ -1566,7 +1557,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>85</v>
       </c>
@@ -1585,9 +1576,9 @@
       <c r="F20" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9b495e2-5989-11e6-a4be-ac72891c3257.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>89</v>
@@ -1602,7 +1593,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>92</v>
       </c>
@@ -1621,9 +1612,9 @@
       <c r="F22" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H22" s="0" t="s">
         <v>97</v>
@@ -1638,7 +1629,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>100</v>
       </c>
@@ -1657,9 +1648,9 @@
       <c r="F24" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cfe4bddb7dbbfc57c19837e7f99d2dda.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H24" s="0" t="s">
         <v>104</v>
@@ -1674,7 +1665,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>100</v>
       </c>
@@ -1693,9 +1684,9 @@
       <c r="F25" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a640b0-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>111</v>
@@ -1710,7 +1701,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>100</v>
       </c>
@@ -1729,9 +1720,9 @@
       <c r="F26" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a673b4-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>116</v>
@@ -1746,7 +1737,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>100</v>
       </c>
@@ -1765,9 +1756,9 @@
       <c r="F27" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a56fd2-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H27" s="0" t="s">
         <v>120</v>
@@ -1782,7 +1773,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>100</v>
       </c>
@@ -1801,9 +1792,9 @@
       <c r="F28" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="G28" s="0" t="n">
+      <c r="G28" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H28" s="0" t="s">
         <v>125</v>
@@ -1818,7 +1809,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>127</v>
       </c>
@@ -1837,9 +1828,9 @@
       <c r="F30" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G30" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>131</v>
@@ -1854,7 +1845,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>127</v>
       </c>
@@ -1873,9 +1864,9 @@
       <c r="F31" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="G31" s="0" t="n">
+      <c r="G31" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>138</v>
@@ -1890,7 +1881,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>127</v>
       </c>
@@ -1909,9 +1900,9 @@
       <c r="F32" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="G32" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H32" s="0" t="s">
         <v>142</v>
@@ -1926,7 +1917,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>127</v>
       </c>
@@ -1945,9 +1936,9 @@
       <c r="F33" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="G33" s="0" t="n">
+      <c r="G33" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H33" s="0" t="s">
         <v>146</v>
@@ -1962,7 +1953,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>127</v>
       </c>
@@ -1981,9 +1972,9 @@
       <c r="F34" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="G34" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H34" s="0" t="s">
         <v>151</v>
@@ -1998,7 +1989,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>127</v>
       </c>
@@ -2017,9 +2008,9 @@
       <c r="F35" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="G35" s="0" t="n">
+      <c r="G35" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H35" s="0" t="s">
         <v>157</v>
@@ -2034,7 +2025,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>127</v>
       </c>
@@ -2053,9 +2044,9 @@
       <c r="F36" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="G36" s="0" t="n">
+      <c r="G36" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H36" s="0" t="s">
         <v>162</v>
@@ -2070,7 +2061,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>164</v>
       </c>
@@ -2089,9 +2080,9 @@
       <c r="F38" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="0" t="n">
+      <c r="G38" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H38" s="0" t="s">
         <v>34</v>
@@ -2106,7 +2097,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>164</v>
       </c>
@@ -2125,9 +2116,9 @@
       <c r="F39" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="0" t="n">
+      <c r="G39" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H39" s="0" t="s">
         <v>41</v>
@@ -2142,7 +2133,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>164</v>
       </c>
@@ -2161,9 +2152,9 @@
       <c r="F40" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G40" s="0" t="n">
+      <c r="G40" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H40" s="0" t="s">
         <v>46</v>
@@ -2178,7 +2169,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>164</v>
       </c>
@@ -2197,9 +2188,9 @@
       <c r="F41" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="0" t="n">
+      <c r="G41" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H41" s="0" t="s">
         <v>51</v>
@@ -2214,7 +2205,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>164</v>
       </c>
@@ -2233,9 +2224,9 @@
       <c r="F42" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="0" t="n">
+      <c r="G42" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H42" s="0" t="s">
         <v>55</v>
@@ -2250,7 +2241,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>164</v>
       </c>
@@ -2269,9 +2260,9 @@
       <c r="F43" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G43" s="0" t="n">
+      <c r="G43" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H43" s="0" t="s">
         <v>60</v>
@@ -2286,7 +2277,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>164</v>
       </c>
@@ -2305,9 +2296,9 @@
       <c r="F44" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="G44" s="0" t="n">
+      <c r="G44" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H44" s="0" t="s">
         <v>66</v>
@@ -2322,7 +2313,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>166</v>
       </c>
@@ -2341,9 +2332,9 @@
       <c r="F46" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G46" s="0" t="n">
+      <c r="G46" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H46" s="0" t="s">
         <v>41</v>
@@ -2358,7 +2349,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>166</v>
       </c>
@@ -2377,9 +2368,9 @@
       <c r="F47" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G47" s="0" t="n">
+      <c r="G47" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H47" s="0" t="s">
         <v>46</v>
@@ -2394,7 +2385,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>166</v>
       </c>
@@ -2413,9 +2404,9 @@
       <c r="F48" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G48" s="0" t="n">
+      <c r="G48" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H48" s="0" t="s">
         <v>51</v>
@@ -2430,7 +2421,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>166</v>
       </c>
@@ -2449,9 +2440,9 @@
       <c r="F49" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G49" s="0" t="n">
+      <c r="G49" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H49" s="0" t="s">
         <v>55</v>
@@ -2466,7 +2457,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>166</v>
       </c>
@@ -2485,9 +2476,9 @@
       <c r="F50" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="G50" s="0" t="n">
+      <c r="G50" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H50" s="0" t="s">
         <v>125</v>
@@ -2502,7 +2493,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>166</v>
       </c>
@@ -2521,9 +2512,9 @@
       <c r="F51" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="G51" s="0" t="n">
+      <c r="G51" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H51" s="0" t="s">
         <v>176</v>
@@ -2538,48 +2529,84 @@
         <v>172</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>178</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>68</v>
+        <v>179</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>179</v>
+        <v>13</v>
       </c>
       <c r="D53" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="E53" s="0" t="s">
-        <v>70</v>
-      </c>
       <c r="F53" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="G53" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="G53" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
+        <v>web</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>72</v>
+        <v>181</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>70</v>
+        <v>182</v>
       </c>
       <c r="K53" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I54" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K54" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>13</v>
@@ -2588,418 +2615,396 @@
         <v>32</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G55" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
-        <v>0</v>
+      <c r="G55" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
+        <v>web</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I55" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="K55" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F56" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="H63" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="I63" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="K63" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="F64" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G56" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H56" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I56" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J56" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K56" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="F57" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G57" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H57" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="I57" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J57" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="K57" s="0" t="s">
+      <c r="G64" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="H64" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="K64" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G65" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="B65" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="F65" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G65" s="0" t="s">
-        <v>193</v>
-      </c>
       <c r="H65" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>195</v>
+        <v>98</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="K65" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="G68" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="B66" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66" s="0" t="s">
+      <c r="H68" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="I68" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="J68" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="K68" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="H69" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="I69" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="K69" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="H72" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="I72" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="J72" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="K72" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="H75" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="I75" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J75" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="E66" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="F66" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G66" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="H66" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="I66" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="J66" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="K66" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="F67" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G67" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="H67" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="I67" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="J67" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="K67" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="B70" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="F70" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="G70" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="H70" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="I70" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="J70" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="K70" s="0" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="F71" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="G71" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="H71" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="I71" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="J71" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="K71" s="0" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="B74" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="E74" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="F74" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="G74" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="H74" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="I74" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="J74" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="K74" s="0" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="K75" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C77" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="B77" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="D77" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="E77" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E77" s="0" t="s">
-        <v>183</v>
-      </c>
       <c r="F77" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G77" s="0" t="s">
-        <v>193</v>
+        <v>228</v>
+      </c>
+      <c r="G77" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="I77" s="0" t="s">
-        <v>18</v>
+        <v>229</v>
       </c>
       <c r="J77" s="0" t="s">
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="K77" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="G78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="J78" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="K78" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>127</v>
+        <v>21</v>
       </c>
       <c r="B79" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="F79" s="0" t="s">
         <v>228</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="D79" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="E79" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="F79" s="0" t="s">
-        <v>231</v>
       </c>
       <c r="G79" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="J79" s="0" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="K79" s="0" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>127</v>
+        <v>21</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>219</v>
+        <v>23</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>231</v>
+        <v>25</v>
       </c>
       <c r="G80" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="J80" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="K80" s="0" t="s">
         <v>29</v>
@@ -3010,143 +3015,61 @@
         <v>21</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>23</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>231</v>
+        <v>25</v>
       </c>
       <c r="G81" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="J81" s="0" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="K81" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B82" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E82" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="F82" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="G82" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H82" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="J82" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="K82" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B83" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E83" s="0" t="s">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="F83" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="G83" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H83" s="0" t="s">
+      <c r="H84" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="J83" s="0" t="s">
+      <c r="I84" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="K83" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="H86" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="I86" s="0" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="H87" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="I87" s="0" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="H88" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="I88" s="0" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B85" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H85" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="I85" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
restored original xls to check if modifications work
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="246">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -85,6 +85,33 @@
     <t xml:space="preserve">CMIP,ISMIP6</t>
   </si>
   <si>
+    <t xml:space="preserve">EmonZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tntc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latitude plev39 time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tendency of Air Temperature Due to Convection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.105                                                                   part of MFP3D        Available in IFS: T-tendency from convection : grib 128.105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twan, Thomas &amp; Gijs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tendencies from cumulus convection scheme.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DynVarMIP,VolMIP</t>
+  </si>
+  <si>
     <t xml:space="preserve">CFmon</t>
   </si>
   <si>
@@ -214,9 +241,6 @@
     <t xml:space="preserve">Grib 126.94 + 126.99 + 126.106 + 126.110       part of MFP3D        Adding all the q-tendencies, thus: grib 128.94 + 128.99 + 128.106 + 128.110.  Alternatively, in IFS: just estimating the delta q per month. So far no direct grib code for the totoal q-tendency found</t>
   </si>
   <si>
-    <t xml:space="preserve">Twan, Thomas &amp; Gijs</t>
-  </si>
-  <si>
     <t xml:space="preserve">AerChemMIP,CFMIP,DAMIP,GeoMIP,HighResMIP,PMIP</t>
   </si>
   <si>
@@ -229,9 +253,6 @@
     <t xml:space="preserve">grib 126.106                                                                   part of MFP3D        Available in IFS: q-tendency from convection: grib 128.106</t>
   </si>
   <si>
-    <t xml:space="preserve">Tendencies from cumulus convection scheme.</t>
-  </si>
-  <si>
     <t xml:space="preserve">tnhusmp</t>
   </si>
   <si>
@@ -242,18 +263,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tendency of specific humidity due to model physics. This includes sources and sinks from parametrized moist physics (e.g. convection, boundary layer, stratiform condensation/evaporation, etc.) and excludes sources and sinks from resolved dynamics or from horizontal or vertical numerical diffusion not associated with model physics.  For example any diffusive mixing by the boundary layer scheme would be included.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tntc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tendency of Air Temperature Due to Convection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K s-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grib 126.105                                                                   part of MFP3D        Available in IFS: T-tendency from convection : grib 128.105</t>
   </si>
   <si>
     <t xml:space="preserve">tntr</t>
@@ -744,6 +753,60 @@
   </si>
   <si>
     <t xml:space="preserve">longitude latitude time typeli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vtendnogw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northward Acceleration Due to Non-Orographic Gravity Wave Drag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m s-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemeted in EC-Earth table 126: grib code 122.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tendency of the northward wind by parameterized nonorographic gravity waves.  (Note that CF name tables only have a general northward tendency for all gravity waves, and we need it separated by type.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vtendogw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northward Acceleration Due to Orographic Gravity Wave Drag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemeted in EC-Earth table 126: grib code 123.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tendency of the northward wind by parameterized orographic gravity waves.  (Note that CF name tables only have a general northward tendency for all gravity waves, and we need it separated by type.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tntnogw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature Tendency Due to Non-Orographic Gravity Wave Dissipation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemeted in EC-Earth table 126: grib code 131.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature tendency due to dissipation of parameterized nonorographic gravity waves.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tntogw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature Tendency Due to Orographic Gravity Wave Dissipation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemeted in EC-Earth table 126: grib code 132.126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature tendency due to dissipation of parameterized orographic gravity waves.</t>
   </si>
   <si>
     <t xml:space="preserve">reffclws</t>
@@ -933,25 +996,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K65536"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="83.6071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.2908163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="83.6071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.2908163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="207.974489795918"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="83.6071428571429"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="80.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,1477 +1089,1477 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="0" t="s">
+      <c r="C5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H6" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="G5" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/52f043533a691ca5721460e316c3a328.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="I5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="J5" s="0" t="s">
         <v>28</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G7" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
         <v>web</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
         <v>web</v>
       </c>
       <c r="H8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
         <v>web</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
         <v>web</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
         <v>web</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="G12" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
         <v>web</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G13" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
         <v>web</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="G14" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d576b3fc447c37d782926441428ffd.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
         <v>web</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E15" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="G15" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6e30ba1e2c19dcbd85faa176d4eae596.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d576b3fc447c37d782926441428ffd.html","web")</f>
         <v>web</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="J15" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G16" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/52f043533a691ca5721460e316c3a328.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6e30ba1e2c19dcbd85faa176d4eae596.html","web")</f>
         <v>web</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="G17" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/52f043533a691ca5721460e316c3a328.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/93a0ba1f23bfc41b720ea68951d28144.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H17" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19" s="0" t="s">
+      <c r="H18" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="0" t="s">
+      <c r="I18" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="G19" s="0" t="str">
+      <c r="E20" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9b495e2-5989-11e6-a4be-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H19" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="I19" s="0" t="s">
+      <c r="H20" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="I20" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" s="0" t="s">
+      <c r="J20" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="K20" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="E21" s="0" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="B22" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="G21" s="0" t="str">
+      <c r="C22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G22" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H21" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="H22" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="I22" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="0" t="s">
+      <c r="J22" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="F23" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cfe4bddb7dbbfc57c19837e7f99d2dda.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>104</v>
+      <c r="K22" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cfe4bddb7dbbfc57c19837e7f99d2dda.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="I24" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="0" t="s">
+      <c r="J24" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="K24" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="G24" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a640b0-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="K24" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="G25" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a640b0-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H25" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="0" t="s">
+      <c r="I25" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="J25" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="F25" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a673b4-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H25" s="0" t="s">
+      <c r="K25" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="J25" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="K25" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="0" t="s">
+      <c r="F26" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a673b4-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H26" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="F26" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a56fd2-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H26" s="0" t="s">
+      <c r="I26" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="J26" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="I26" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>118</v>
-      </c>
       <c r="K26" s="0" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a56fd2-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H27" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="0" t="s">
+      <c r="I27" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="J27" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="F27" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G27" s="0" t="str">
+      <c r="K27" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="G28" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H27" s="0" t="s">
+      <c r="H28" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="K28" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="G29" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="J29" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="K29" s="0" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="G30" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="I30" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="0" t="s">
+      <c r="J30" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="K30" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="G30" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="J30" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="K30" s="0" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="F31" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="0" t="s">
+      <c r="G31" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H31" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="F31" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="G31" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H31" s="0" t="s">
+      <c r="I31" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J31" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="I31" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="J31" s="0" t="s">
-        <v>140</v>
-      </c>
       <c r="K31" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="0" t="s">
+      <c r="F32" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="G32" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H32" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="I32" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="K32" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="G32" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="J32" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="K32" s="0" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="0" t="s">
+      <c r="F33" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G33" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H33" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="I33" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J33" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="F33" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="I33" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="J33" s="0" t="s">
-        <v>149</v>
-      </c>
       <c r="K33" s="0" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H34" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="C34" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="0" t="s">
+      <c r="I34" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="J34" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="K34" s="0" t="s">
         <v>153</v>
-      </c>
-      <c r="G34" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="J34" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="K34" s="0" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="G35" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H35" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="0" t="s">
+      <c r="I35" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J35" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="F35" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="G35" s="0" t="str">
+      <c r="K35" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="G36" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H35" s="0" t="s">
+      <c r="H36" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="K36" s="0" t="s">
         <v>159</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="J35" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="K35" s="0" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J37" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="K37" s="0" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G38" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bb4d31072e09cd4935f1c20a2c533bbd.html","web")</f>
         <v>web</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K38" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G39" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
         <v>web</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G40" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
         <v>web</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K40" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G41" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
         <v>web</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="K41" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G42" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
         <v>web</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="K42" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="G43" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b045cae1f65ba99831648f136b309e91.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G44" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/987be9b68c051baf4f0c5b6e8c26b4d8.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H43" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="I43" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J43" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="K43" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G45" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="I45" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J45" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="K45" s="0" t="s">
+      <c r="H44" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="K44" s="0" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F46" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G46" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7308096ae00ff52340909b2a59415f82.html","web")</f>
         <v>web</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="K46" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F47" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G47" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0bbbf303ac691061a69938846f32b23b.html","web")</f>
         <v>web</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K47" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G48" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe9d4b45792f7d6430fe2a9c9b7234b1.html","web")</f>
         <v>web</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>120</v>
+        <v>53</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ce9ab9b945fcc86013ad10431d8f252e.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="K49" s="0" t="s">
         <v>168</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G49" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H49" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="I49" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="J49" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="K49" s="0" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>170</v>
+        <v>123</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E50" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="G50" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="K50" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="F50" s="0" t="s">
+      <c r="E51" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="G51" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="K51" s="0" t="s">
         <v>172</v>
-      </c>
-      <c r="G50" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H50" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="I50" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="J50" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="K50" s="0" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H52" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="I52" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J52" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="K52" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>12</v>
+        <v>179</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>15</v>
+        <v>180</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G53" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
         <v>web</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>17</v>
+        <v>181</v>
       </c>
       <c r="I53" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>19</v>
+        <v>182</v>
       </c>
       <c r="K53" s="0" t="s">
         <v>20</v>
@@ -2503,319 +2567,509 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>181</v>
+        <v>15</v>
       </c>
       <c r="F54" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G54" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>182</v>
+        <v>17</v>
       </c>
       <c r="I54" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J54" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K54" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B55" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="K54" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="C55" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="F55" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H55" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="C62" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" s="0" t="s">
+      <c r="I55" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="K55" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="G62" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="H62" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="I62" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="J62" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="K62" s="0" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D63" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="H63" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="E63" s="0" t="s">
+      <c r="I63" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="F63" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G63" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="H63" s="0" t="s">
+      <c r="J63" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="I63" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="J63" s="0" t="s">
-        <v>194</v>
-      </c>
       <c r="K63" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>12</v>
+        <v>179</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D64" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="E64" s="0" t="s">
         <v>195</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>196</v>
       </c>
       <c r="F64" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G64" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="H64" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="K64" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="H64" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="I64" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="J64" s="0" t="s">
+      <c r="B65" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="K64" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="E65" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="F65" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="H65" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="C67" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E67" s="0" t="s">
+      <c r="I65" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J65" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="F67" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="G67" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="H67" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="I67" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="J67" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="K67" s="0" t="s">
-        <v>206</v>
+      <c r="K65" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B68" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="H68" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="I68" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="C68" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E68" s="0" t="s">
+      <c r="J68" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="F68" s="0" t="s">
+      <c r="K68" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="G68" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="H68" s="0" t="s">
+      <c r="B69" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="H69" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="I69" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="K69" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="I68" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="J68" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="K68" s="0" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="E71" s="0" t="s">
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="F71" s="0" t="s">
+      <c r="B72" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="G71" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="H71" s="0" t="s">
+      <c r="C72" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="I71" s="0" t="s">
+      <c r="E72" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="J71" s="0" t="s">
+      <c r="F72" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="K71" s="0" t="s">
+      <c r="G72" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="H72" s="0" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="I72" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="B74" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D74" s="0" t="s">
+      <c r="J72" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="E74" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="F74" s="0" t="s">
+      <c r="K72" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="F75" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G74" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="H74" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="I74" s="0" t="s">
+      <c r="G75" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="H75" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="I75" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="J74" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="K74" s="0" t="s">
+      <c r="J75" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="K75" s="0" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="G77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="J77" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="K77" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>222</v>
+        <v>127</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="G78" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="I78" s="0" t="s">
-        <v>189</v>
+        <v>233</v>
+      </c>
+      <c r="J78" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="K78" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>222</v>
+        <v>21</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="G79" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="I79" s="0" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>229</v>
+      </c>
+      <c r="J79" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="K79" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="J80" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="K80" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="J81" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="K81" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H84" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="I84" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H85" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="I85" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2830,7 +3084,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>